<commit_message>
Both hybrid pile funcs added and tested
</commit_message>
<xml_diff>
--- a/Input/PDAcalc.xlsx
+++ b/Input/PDAcalc.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8E88DD-B68D-4D70-8CE0-1A982139A43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9955DFB-4568-4B6F-BC46-2792224CC617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCATIONS" sheetId="66" r:id="rId1"/>
@@ -770,7 +770,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="285">
   <si>
     <t>Setting</t>
   </si>
@@ -1053,9 +1053,6 @@
     <t>line</t>
   </si>
   <si>
-    <t>dash</t>
-  </si>
-  <si>
     <t>AO1</t>
   </si>
   <si>
@@ -1110,15 +1107,9 @@
     <t>CPTProfile</t>
   </si>
   <si>
-    <t>Blow_Count_HB</t>
-  </si>
-  <si>
     <t>Fatigue_UB</t>
   </si>
   <si>
-    <t>Reduced energy</t>
-  </si>
-  <si>
     <t>ituotdao1db</t>
   </si>
   <si>
@@ -1242,9 +1233,6 @@
     <t xml:space="preserve">Emb L </t>
   </si>
   <si>
-    <t>Full energy</t>
-  </si>
-  <si>
     <t>Switch</t>
   </si>
   <si>
@@ -1290,9 +1278,6 @@
     <t>Fatigue calculation</t>
   </si>
   <si>
-    <t>Analysis option 1</t>
-  </si>
-  <si>
     <t>SPSO</t>
   </si>
   <si>
@@ -1401,22 +1386,10 @@
     <t>Jones</t>
   </si>
   <si>
-    <t>NMS</t>
-  </si>
-  <si>
-    <t>CPT PDA profile</t>
-  </si>
-  <si>
     <t>NoiseSTR_4000</t>
   </si>
   <si>
     <t>NoiseSTR_5500</t>
-  </si>
-  <si>
-    <t>S-5500</t>
-  </si>
-  <si>
-    <t>S-4000</t>
   </si>
   <si>
     <t>Full_UB_4000</t>
@@ -1652,6 +1625,9 @@
   </si>
   <si>
     <t>Depth</t>
+  </si>
+  <si>
+    <t>Hybrid option 1</t>
   </si>
 </sst>
 </file>
@@ -2398,7 +2374,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2730,6 +2706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3486,7 +3463,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3511,80 +3488,80 @@
   <sheetData>
     <row r="1" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="116" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B1" s="116" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="140" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="140" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1" s="140" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="140" t="s">
+        <v>246</v>
+      </c>
+      <c r="G1" s="140" t="s">
+        <v>247</v>
+      </c>
+      <c r="H1" s="140" t="s">
+        <v>248</v>
+      </c>
+      <c r="I1" s="140" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1" s="140" t="s">
+        <v>250</v>
+      </c>
+      <c r="K1" s="140" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="140" t="s">
+      <c r="L1" s="140" t="s">
         <v>252</v>
       </c>
-      <c r="D1" s="140" t="s">
+      <c r="M1" s="140" t="s">
         <v>253</v>
       </c>
-      <c r="E1" s="140" t="s">
+      <c r="N1" s="140" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="140" t="s">
+      <c r="O1" s="140" t="s">
         <v>255</v>
       </c>
-      <c r="G1" s="140" t="s">
+      <c r="P1" s="141" t="s">
         <v>256</v>
       </c>
-      <c r="H1" s="140" t="s">
+      <c r="Q1" s="140" t="s">
         <v>257</v>
       </c>
-      <c r="I1" s="140" t="s">
+      <c r="R1" s="140" t="s">
         <v>258</v>
       </c>
-      <c r="J1" s="140" t="s">
+      <c r="S1" s="140" t="s">
         <v>259</v>
       </c>
-      <c r="K1" s="140" t="s">
+      <c r="T1" s="140" t="s">
         <v>260</v>
       </c>
-      <c r="L1" s="140" t="s">
+      <c r="U1" s="140" t="s">
         <v>261</v>
       </c>
-      <c r="M1" s="140" t="s">
+      <c r="V1" s="140" t="s">
         <v>262</v>
-      </c>
-      <c r="N1" s="140" t="s">
-        <v>263</v>
-      </c>
-      <c r="O1" s="140" t="s">
-        <v>264</v>
-      </c>
-      <c r="P1" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q1" s="140" t="s">
-        <v>266</v>
-      </c>
-      <c r="R1" s="140" t="s">
-        <v>267</v>
-      </c>
-      <c r="S1" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="T1" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="U1" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="V1" s="140" t="s">
-        <v>271</v>
       </c>
       <c r="W1" s="116" t="s">
         <v>79</v>
       </c>
       <c r="X1" s="113"/>
       <c r="AC1" s="137" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AD1" s="138" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AE1" s="139" t="s">
         <v>79</v>
@@ -3604,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="100" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C2" s="129">
         <v>70</v>
@@ -3690,7 +3667,7 @@
       </c>
       <c r="X2" s="72"/>
       <c r="AC2" s="134" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="AD2" s="135">
         <v>70</v>
@@ -5302,7 +5279,7 @@
       <c r="V50" s="131"/>
       <c r="W50" s="35"/>
       <c r="X50" s="72" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.3">
@@ -5512,7 +5489,7 @@
       <c r="V58" s="131"/>
       <c r="W58" s="35"/>
       <c r="X58" s="72" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.3">
@@ -5930,7 +5907,7 @@
       <c r="V74" s="131"/>
       <c r="W74" s="35"/>
       <c r="X74" s="72" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.3">
@@ -6878,7 +6855,7 @@
       <c r="V110" s="129"/>
       <c r="W110" s="130"/>
       <c r="X110" s="128" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.3">
@@ -8211,8 +8188,8 @@
   </sheetPr>
   <dimension ref="A1:AB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X29" sqref="X29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8241,7 +8218,7 @@
     <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:26" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="105" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C2" s="106" t="s">
         <v>35</v>
@@ -8256,23 +8233,23 @@
         <v>37</v>
       </c>
       <c r="G2" s="148" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="H2" s="149" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I2" s="148" t="s">
-        <v>171</v>
-      </c>
-      <c r="K2" s="179" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="180" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="180"/>
+      <c r="L2" s="181"/>
       <c r="M2" s="53"/>
-      <c r="N2" s="179" t="s">
-        <v>227</v>
-      </c>
-      <c r="O2" s="180"/>
+      <c r="N2" s="180" t="s">
+        <v>218</v>
+      </c>
+      <c r="O2" s="181"/>
     </row>
     <row r="3" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="13">
@@ -8305,11 +8282,11 @@
         <v>39</v>
       </c>
       <c r="L3" s="47" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M3" s="53"/>
       <c r="N3" s="31" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="O3" s="27">
         <v>0</v>
@@ -8349,7 +8326,7 @@
         <v>40</v>
       </c>
       <c r="L4" s="48" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="M4" s="53"/>
       <c r="N4" s="19" t="s">
@@ -8369,7 +8346,7 @@
         <v>Full_UB_5500</v>
       </c>
       <c r="D5" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="54">
         <f t="shared" si="1"/>
@@ -8391,14 +8368,14 @@
         <v>38</v>
       </c>
       <c r="L5" s="48" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="M5" s="53"/>
       <c r="N5" s="31" t="s">
         <v>9</v>
       </c>
       <c r="O5" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.3">
@@ -8430,10 +8407,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="L6" s="48" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="M6" s="53"/>
     </row>
@@ -8466,10 +8443,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="56" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
@@ -8504,7 +8481,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="L8" s="47">
         <v>0</v>
@@ -8540,7 +8517,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="L9" s="48"/>
       <c r="M9" s="53"/>
@@ -8574,7 +8551,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="L10" s="48">
         <v>1000</v>
@@ -8610,7 +8587,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="L11" s="48">
         <v>0</v>
@@ -8647,10 +8624,10 @@
         <v>0</v>
       </c>
       <c r="K12" s="56" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="M12" s="53"/>
     </row>
@@ -8749,10 +8726,10 @@
       <c r="G16" s="54"/>
       <c r="H16" s="54"/>
       <c r="I16" s="34"/>
-      <c r="K16" s="179" t="s">
-        <v>217</v>
-      </c>
-      <c r="L16" s="180"/>
+      <c r="K16" s="180" t="s">
+        <v>208</v>
+      </c>
+      <c r="L16" s="181"/>
     </row>
     <row r="17" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="str">
@@ -8772,11 +8749,11 @@
       <c r="K17" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>288</v>
+      <c r="L17" s="177" t="s">
+        <v>279</v>
       </c>
       <c r="P17" s="53" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:28" s="53" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8795,10 +8772,10 @@
       <c r="H18" s="54"/>
       <c r="I18" s="34"/>
       <c r="K18" s="56" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.3">
@@ -8873,42 +8850,42 @@
     </row>
     <row r="23" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="177" t="s">
+      <c r="B24" s="178" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="184"/>
-      <c r="D24" s="184"/>
-      <c r="E24" s="184"/>
-      <c r="F24" s="184"/>
-      <c r="G24" s="184"/>
-      <c r="H24" s="184"/>
-      <c r="I24" s="184"/>
-      <c r="J24" s="184"/>
-      <c r="K24" s="184"/>
-      <c r="L24" s="184"/>
-      <c r="M24" s="184"/>
-      <c r="N24" s="184"/>
-      <c r="O24" s="184"/>
-      <c r="P24" s="184"/>
-      <c r="Q24" s="184"/>
-      <c r="R24" s="184"/>
-      <c r="S24" s="184"/>
-      <c r="T24" s="184"/>
-      <c r="U24" s="184"/>
-      <c r="V24" s="184"/>
-      <c r="W24" s="184"/>
-      <c r="X24" s="184"/>
-      <c r="Y24" s="184"/>
-      <c r="Z24" s="184"/>
-      <c r="AA24" s="184"/>
-      <c r="AB24" s="178"/>
+      <c r="C24" s="185"/>
+      <c r="D24" s="185"/>
+      <c r="E24" s="185"/>
+      <c r="F24" s="185"/>
+      <c r="G24" s="185"/>
+      <c r="H24" s="185"/>
+      <c r="I24" s="185"/>
+      <c r="J24" s="185"/>
+      <c r="K24" s="185"/>
+      <c r="L24" s="185"/>
+      <c r="M24" s="185"/>
+      <c r="N24" s="185"/>
+      <c r="O24" s="185"/>
+      <c r="P24" s="185"/>
+      <c r="Q24" s="185"/>
+      <c r="R24" s="185"/>
+      <c r="S24" s="185"/>
+      <c r="T24" s="185"/>
+      <c r="U24" s="185"/>
+      <c r="V24" s="185"/>
+      <c r="W24" s="185"/>
+      <c r="X24" s="185"/>
+      <c r="Y24" s="185"/>
+      <c r="Z24" s="185"/>
+      <c r="AA24" s="185"/>
+      <c r="AB24" s="179"/>
     </row>
     <row r="25" spans="1:28" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="143" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C25" s="144" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D25" s="144" t="s">
         <v>1</v>
@@ -8929,10 +8906,10 @@
         <v>45</v>
       </c>
       <c r="J25" s="144" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K25" s="144" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L25" s="144" t="s">
         <v>31</v>
@@ -8959,31 +8936,31 @@
         <v>65</v>
       </c>
       <c r="T25" s="144" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="U25" s="144" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="V25" s="144" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="W25" s="144" t="s">
         <v>77</v>
       </c>
       <c r="X25" s="144" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="Y25" s="144" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Z25" s="144" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA25" s="144" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AB25" s="145" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.3">
@@ -8992,7 +8969,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="142" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D26" s="142">
         <v>0</v>
@@ -9032,13 +9009,13 @@
         <v>1</v>
       </c>
       <c r="Q26" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R26" s="142">
         <v>1</v>
       </c>
       <c r="S26" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T26" s="142">
         <v>300</v>
@@ -9075,7 +9052,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="142" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D27" s="142">
         <v>0</v>
@@ -9115,13 +9092,13 @@
         <v>1</v>
       </c>
       <c r="Q27" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R27" s="142">
         <v>1</v>
       </c>
       <c r="S27" s="142" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T27" s="142">
         <v>0</v>
@@ -9148,7 +9125,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="150">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
@@ -9158,7 +9135,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="142" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D28" s="142">
         <v>0</v>
@@ -9198,13 +9175,13 @@
         <v>1</v>
       </c>
       <c r="Q28" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R28" s="142">
         <v>1</v>
       </c>
       <c r="S28" s="142" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T28" s="142">
         <v>0</v>
@@ -9231,7 +9208,7 @@
         <v>0</v>
       </c>
       <c r="AB28" s="150">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
@@ -9241,7 +9218,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="142" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D29" s="142">
         <v>0</v>
@@ -9281,13 +9258,13 @@
         <v>1</v>
       </c>
       <c r="Q29" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R29" s="142">
         <v>1</v>
       </c>
       <c r="S29" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T29" s="142">
         <v>0</v>
@@ -9324,7 +9301,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="142" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D30" s="142">
         <v>0</v>
@@ -9364,13 +9341,13 @@
         <v>1</v>
       </c>
       <c r="Q30" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R30" s="142">
         <v>1</v>
       </c>
       <c r="S30" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T30" s="142">
         <v>0</v>
@@ -9382,7 +9359,7 @@
         <v>3411.4</v>
       </c>
       <c r="W30" s="142" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X30" s="142" t="s">
         <v>91</v>
@@ -9407,7 +9384,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="142" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D31" s="142">
         <v>0</v>
@@ -9447,13 +9424,13 @@
         <v>1</v>
       </c>
       <c r="Q31" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R31" s="142">
         <v>1</v>
       </c>
       <c r="S31" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T31" s="142">
         <v>0</v>
@@ -9490,7 +9467,7 @@
         <v>7</v>
       </c>
       <c r="C32" s="142" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D32" s="142">
         <v>0</v>
@@ -9530,13 +9507,13 @@
         <v>1</v>
       </c>
       <c r="Q32" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R32" s="142">
         <v>1</v>
       </c>
       <c r="S32" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T32" s="142">
         <v>0</v>
@@ -9573,7 +9550,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="142" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D33" s="142">
         <v>0</v>
@@ -9613,13 +9590,13 @@
         <v>1</v>
       </c>
       <c r="Q33" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R33" s="142">
         <v>1</v>
       </c>
       <c r="S33" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T33" s="142">
         <v>0</v>
@@ -9656,7 +9633,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="142" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D34" s="142">
         <v>0</v>
@@ -9696,13 +9673,13 @@
         <v>1</v>
       </c>
       <c r="Q34" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R34" s="142">
         <v>1</v>
       </c>
       <c r="S34" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T34" s="142">
         <v>300</v>
@@ -9739,7 +9716,7 @@
         <v>10</v>
       </c>
       <c r="C35" s="142" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D35" s="142">
         <v>0</v>
@@ -9779,13 +9756,13 @@
         <v>1</v>
       </c>
       <c r="Q35" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R35" s="142">
         <v>1</v>
       </c>
       <c r="S35" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T35" s="142">
         <v>300</v>
@@ -9822,7 +9799,7 @@
         <v>11</v>
       </c>
       <c r="C36" s="142" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D36" s="142">
         <v>0</v>
@@ -9862,13 +9839,13 @@
         <v>1</v>
       </c>
       <c r="Q36" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R36" s="142">
         <v>1</v>
       </c>
       <c r="S36" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T36" s="142">
         <v>0</v>
@@ -9905,7 +9882,7 @@
         <v>12</v>
       </c>
       <c r="C37" s="142" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D37" s="142">
         <v>0</v>
@@ -9945,13 +9922,13 @@
         <v>1</v>
       </c>
       <c r="Q37" s="142" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="R37" s="142">
         <v>1</v>
       </c>
       <c r="S37" s="142" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T37" s="142">
         <v>0</v>
@@ -10247,28 +10224,28 @@
     </row>
     <row r="46" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="47" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="181" t="s">
+      <c r="B47" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="182"/>
-      <c r="D47" s="182"/>
-      <c r="E47" s="182"/>
-      <c r="F47" s="182"/>
-      <c r="G47" s="182"/>
-      <c r="H47" s="183"/>
-      <c r="J47" s="181" t="s">
+      <c r="C47" s="183"/>
+      <c r="D47" s="183"/>
+      <c r="E47" s="183"/>
+      <c r="F47" s="183"/>
+      <c r="G47" s="183"/>
+      <c r="H47" s="184"/>
+      <c r="J47" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="K47" s="182"/>
-      <c r="L47" s="182"/>
-      <c r="M47" s="182"/>
-      <c r="N47" s="182"/>
-      <c r="O47" s="182"/>
-      <c r="P47" s="182"/>
-      <c r="Q47" s="182"/>
-      <c r="R47" s="182"/>
-      <c r="S47" s="182"/>
-      <c r="T47" s="183"/>
+      <c r="K47" s="183"/>
+      <c r="L47" s="183"/>
+      <c r="M47" s="183"/>
+      <c r="N47" s="183"/>
+      <c r="O47" s="183"/>
+      <c r="P47" s="183"/>
+      <c r="Q47" s="183"/>
+      <c r="R47" s="183"/>
+      <c r="S47" s="183"/>
+      <c r="T47" s="184"/>
     </row>
     <row r="48" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="143" t="s">
@@ -10626,27 +10603,27 @@
     </row>
     <row r="62" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="63" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="177" t="s">
-        <v>131</v>
-      </c>
-      <c r="C63" s="178"/>
-      <c r="E63" s="177" t="s">
-        <v>291</v>
-      </c>
-      <c r="F63" s="178"/>
+      <c r="B63" s="178" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="179"/>
+      <c r="E63" s="178" t="s">
+        <v>282</v>
+      </c>
+      <c r="F63" s="179"/>
     </row>
     <row r="64" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" s="143" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C64" s="145" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E64" s="143" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="F64" s="145" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
@@ -10845,12 +10822,12 @@
   </sheetPr>
   <dimension ref="A1:AT42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="14" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="14" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C17" sqref="C17"/>
       <selection pane="topRight" activeCell="C17" sqref="C17"/>
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10870,17 +10847,17 @@
     <row r="1" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="124"/>
       <c r="D2" s="105" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E2" s="106" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F2" s="105" t="s">
         <v>80</v>
@@ -10888,33 +10865,33 @@
       <c r="G2" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="185" t="s">
+      <c r="H2" s="186" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="185"/>
-      <c r="J2" s="185"/>
-      <c r="K2" s="185"/>
-      <c r="L2" s="185"/>
-      <c r="M2" s="185"/>
-      <c r="N2" s="186"/>
-      <c r="O2" s="187" t="s">
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="186"/>
+      <c r="M2" s="186"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="188" t="s">
         <v>84</v>
       </c>
-      <c r="P2" s="185"/>
-      <c r="Q2" s="185"/>
-      <c r="R2" s="185"/>
-      <c r="S2" s="185"/>
-      <c r="T2" s="185"/>
-      <c r="U2" s="186"/>
-      <c r="V2" s="187" t="s">
+      <c r="P2" s="186"/>
+      <c r="Q2" s="186"/>
+      <c r="R2" s="186"/>
+      <c r="S2" s="186"/>
+      <c r="T2" s="186"/>
+      <c r="U2" s="187"/>
+      <c r="V2" s="188" t="s">
         <v>90</v>
       </c>
-      <c r="W2" s="185"/>
-      <c r="X2" s="185"/>
-      <c r="Y2" s="185"/>
-      <c r="Z2" s="185"/>
-      <c r="AA2" s="185"/>
-      <c r="AB2" s="186"/>
+      <c r="W2" s="186"/>
+      <c r="X2" s="186"/>
+      <c r="Y2" s="186"/>
+      <c r="Z2" s="186"/>
+      <c r="AA2" s="186"/>
+      <c r="AB2" s="187"/>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" s="95">
@@ -10927,7 +10904,7 @@
       </c>
       <c r="C3" s="35"/>
       <c r="D3" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="122">
         <v>1</v>
@@ -10939,22 +10916,18 @@
         <v>86</v>
       </c>
       <c r="H3" s="35">
-        <v>1</v>
-      </c>
-      <c r="I3" s="35">
-        <v>9</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I3" s="35"/>
       <c r="J3" s="35"/>
       <c r="K3" s="35"/>
       <c r="L3" s="35"/>
       <c r="M3" s="35"/>
       <c r="N3" s="30"/>
       <c r="O3" s="110" t="s">
-        <v>214</v>
-      </c>
-      <c r="P3" s="35" t="s">
-        <v>213</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="P3" s="35"/>
       <c r="Q3" s="35"/>
       <c r="R3" s="35"/>
       <c r="S3" s="35"/>
@@ -10963,9 +10936,7 @@
       <c r="V3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="W3" s="54" t="s">
-        <v>93</v>
-      </c>
+      <c r="W3" s="54"/>
       <c r="X3" s="54"/>
       <c r="Y3" s="54"/>
       <c r="Z3" s="54"/>
@@ -10983,35 +10954,31 @@
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="100">
         <f>IF(F4="","",E3+1)</f>
         <v>2</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="G4" s="126" t="s">
         <v>87</v>
       </c>
       <c r="H4" s="35">
-        <v>8</v>
-      </c>
-      <c r="I4" s="35">
-        <v>6</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I4" s="35"/>
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
       <c r="L4" s="35"/>
       <c r="M4" s="35"/>
       <c r="N4" s="34"/>
       <c r="O4" s="110" t="s">
-        <v>78</v>
-      </c>
-      <c r="P4" s="35" t="s">
-        <v>74</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="P4" s="35"/>
       <c r="Q4" s="35"/>
       <c r="R4" s="35"/>
       <c r="S4" s="35"/>
@@ -11020,9 +10987,7 @@
       <c r="V4" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="W4" s="54" t="s">
-        <v>93</v>
-      </c>
+      <c r="W4" s="54"/>
       <c r="X4" s="54"/>
       <c r="Y4" s="54"/>
       <c r="Z4" s="54"/>
@@ -11049,36 +11014,31 @@
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="110">
-        <f t="shared" ref="D5:D40" si="0">IF(E5="","",0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="100">
-        <f t="shared" ref="E5:E40" si="1">IF(F5="","",E4+1)</f>
+        <f t="shared" ref="E5:E40" si="0">IF(F5="","",E4+1)</f>
         <v>3</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>86</v>
+        <v>182</v>
       </c>
       <c r="G5" s="126" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H5" s="35">
-        <v>8</v>
-      </c>
-      <c r="I5" s="35">
-        <v>6</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I5" s="35"/>
       <c r="J5" s="35"/>
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
       <c r="M5" s="35"/>
       <c r="N5" s="34"/>
       <c r="O5" s="110" t="s">
-        <v>78</v>
-      </c>
-      <c r="P5" s="35" t="s">
-        <v>74</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="P5" s="35"/>
       <c r="Q5" s="35"/>
       <c r="R5" s="35"/>
       <c r="S5" s="35"/>
@@ -11087,9 +11047,7 @@
       <c r="V5" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="W5" s="54" t="s">
-        <v>93</v>
-      </c>
+      <c r="W5" s="54"/>
       <c r="X5" s="54"/>
       <c r="Y5" s="54"/>
       <c r="Z5" s="54"/>
@@ -11107,48 +11065,26 @@
         <v>PileRun_UB</v>
       </c>
       <c r="C6" s="35"/>
-      <c r="D6" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="100">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="G6" s="126" t="s">
-        <v>88</v>
-      </c>
-      <c r="H6" s="35">
-        <v>1</v>
-      </c>
-      <c r="I6" s="35">
-        <v>9</v>
-      </c>
+      <c r="D6" s="110"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
       <c r="M6" s="35"/>
       <c r="N6" s="34"/>
-      <c r="O6" s="110" t="s">
-        <v>214</v>
-      </c>
-      <c r="P6" s="35" t="s">
-        <v>213</v>
-      </c>
+      <c r="O6" s="110"/>
+      <c r="P6" s="35"/>
       <c r="Q6" s="35"/>
       <c r="R6" s="35"/>
       <c r="S6" s="35"/>
       <c r="T6" s="35"/>
       <c r="U6" s="34"/>
-      <c r="V6" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="W6" s="54" t="s">
-        <v>93</v>
-      </c>
+      <c r="V6" s="9"/>
+      <c r="W6" s="54"/>
       <c r="X6" s="54"/>
       <c r="Y6" s="54"/>
       <c r="Z6" s="54"/>
@@ -11165,41 +11101,25 @@
         <v>PileRun_LB</v>
       </c>
       <c r="C7" s="35"/>
-      <c r="D7" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="100">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="G7" s="126" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="35">
-        <v>1</v>
-      </c>
+      <c r="D7" s="110"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="35"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
       <c r="N7" s="34"/>
-      <c r="O7" s="110" t="s">
-        <v>209</v>
-      </c>
+      <c r="O7" s="110"/>
       <c r="P7" s="35"/>
       <c r="Q7" s="35"/>
       <c r="R7" s="35"/>
       <c r="S7" s="35"/>
       <c r="T7" s="35"/>
       <c r="U7" s="34"/>
-      <c r="V7" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="V7" s="9"/>
       <c r="W7" s="54"/>
       <c r="X7" s="54"/>
       <c r="Y7" s="54"/>
@@ -11217,48 +11137,26 @@
         <v>Entrapped_UB</v>
       </c>
       <c r="C8" s="35"/>
-      <c r="D8" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="100">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="126" t="s">
-        <v>89</v>
-      </c>
-      <c r="H8" s="35">
-        <v>7</v>
-      </c>
-      <c r="I8" s="35">
-        <v>8</v>
-      </c>
+      <c r="D8" s="110"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
       <c r="M8" s="35"/>
       <c r="N8" s="34"/>
-      <c r="O8" s="110" t="s">
-        <v>114</v>
-      </c>
-      <c r="P8" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="O8" s="110"/>
+      <c r="P8" s="35"/>
       <c r="Q8" s="35"/>
       <c r="R8" s="35"/>
       <c r="S8" s="35"/>
       <c r="T8" s="35"/>
       <c r="U8" s="34"/>
-      <c r="V8" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="W8" s="54" t="s">
-        <v>92</v>
-      </c>
+      <c r="V8" s="9"/>
+      <c r="W8" s="54"/>
       <c r="X8" s="54"/>
       <c r="Y8" s="54"/>
       <c r="Z8" s="54"/>
@@ -11275,48 +11173,26 @@
         <v>Breakdown_BE</v>
       </c>
       <c r="C9" s="35"/>
-      <c r="D9" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="100">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="126" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="35">
-        <v>4</v>
-      </c>
-      <c r="I9" s="35">
-        <v>3</v>
-      </c>
+      <c r="D9" s="110"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
       <c r="M9" s="35"/>
       <c r="N9" s="34"/>
-      <c r="O9" s="110" t="s">
-        <v>114</v>
-      </c>
-      <c r="P9" s="35" t="s">
-        <v>156</v>
-      </c>
+      <c r="O9" s="110"/>
+      <c r="P9" s="35"/>
       <c r="Q9" s="35"/>
       <c r="R9" s="35"/>
       <c r="S9" s="35"/>
       <c r="T9" s="35"/>
       <c r="U9" s="34"/>
-      <c r="V9" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="W9" s="54" t="s">
-        <v>92</v>
-      </c>
+      <c r="V9" s="9"/>
+      <c r="W9" s="54"/>
       <c r="X9" s="54"/>
       <c r="Y9" s="54"/>
       <c r="Z9" s="54"/>
@@ -11333,41 +11209,25 @@
         <v>Entrapped_BE</v>
       </c>
       <c r="C10" s="35"/>
-      <c r="D10" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="100">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="126" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="35">
-        <v>9</v>
-      </c>
+      <c r="D10" s="110"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="35"/>
       <c r="I10" s="35"/>
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35"/>
       <c r="M10" s="35"/>
       <c r="N10" s="34"/>
-      <c r="O10" s="110" t="s">
-        <v>172</v>
-      </c>
+      <c r="O10" s="110"/>
       <c r="P10" s="35"/>
       <c r="Q10" s="35"/>
       <c r="R10" s="35"/>
       <c r="S10" s="35"/>
       <c r="T10" s="35"/>
       <c r="U10" s="34"/>
-      <c r="V10" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="V10" s="9"/>
       <c r="W10" s="54"/>
       <c r="X10" s="54"/>
       <c r="Y10" s="54"/>
@@ -11385,48 +11245,26 @@
         <v>NoiseSTR_5500</v>
       </c>
       <c r="C11" s="35"/>
-      <c r="D11" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="100">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="G11" s="126" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="35">
-        <v>1</v>
-      </c>
-      <c r="I11" s="35">
-        <v>9</v>
-      </c>
+      <c r="D11" s="110"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
       <c r="J11" s="35"/>
       <c r="K11" s="35"/>
       <c r="L11" s="35"/>
       <c r="M11" s="35"/>
       <c r="N11" s="34"/>
-      <c r="O11" s="110" t="s">
-        <v>214</v>
-      </c>
-      <c r="P11" s="35" t="s">
-        <v>213</v>
-      </c>
+      <c r="O11" s="110"/>
+      <c r="P11" s="35"/>
       <c r="Q11" s="35"/>
       <c r="R11" s="35"/>
       <c r="S11" s="35"/>
       <c r="T11" s="35"/>
       <c r="U11" s="34"/>
-      <c r="V11" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="W11" s="54" t="s">
-        <v>93</v>
-      </c>
+      <c r="V11" s="9"/>
+      <c r="W11" s="54"/>
       <c r="X11" s="54"/>
       <c r="Y11" s="54"/>
       <c r="Z11" s="54"/>
@@ -11443,41 +11281,25 @@
         <v>NoiseSTR_ACC_SENSI</v>
       </c>
       <c r="C12" s="35"/>
-      <c r="D12" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="100">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" s="126" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="35">
-        <v>8</v>
-      </c>
+      <c r="D12" s="110"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="126"/>
+      <c r="H12" s="35"/>
       <c r="I12" s="35"/>
       <c r="J12" s="35"/>
       <c r="K12" s="35"/>
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="110" t="s">
-        <v>210</v>
-      </c>
+      <c r="O12" s="110"/>
       <c r="P12" s="35"/>
       <c r="Q12" s="35"/>
       <c r="R12" s="35"/>
       <c r="S12" s="35"/>
       <c r="T12" s="35"/>
       <c r="U12" s="34"/>
-      <c r="V12" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="V12" s="9"/>
       <c r="W12" s="54"/>
       <c r="X12" s="54"/>
       <c r="Y12" s="54"/>
@@ -11495,48 +11317,26 @@
         <v>Fatigue_BLOW</v>
       </c>
       <c r="C13" s="35"/>
-      <c r="D13" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="100">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="G13" s="126" t="s">
-        <v>87</v>
-      </c>
-      <c r="H13" s="35">
-        <v>5</v>
-      </c>
-      <c r="I13" s="35">
-        <v>6</v>
-      </c>
+      <c r="D13" s="110"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="126"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
       <c r="N13" s="34"/>
-      <c r="O13" s="110" t="s">
-        <v>105</v>
-      </c>
-      <c r="P13" s="35" t="s">
-        <v>74</v>
-      </c>
+      <c r="O13" s="110"/>
+      <c r="P13" s="35"/>
       <c r="Q13" s="35"/>
       <c r="R13" s="35"/>
       <c r="S13" s="35"/>
       <c r="T13" s="35"/>
       <c r="U13" s="34"/>
-      <c r="V13" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="W13" s="54" t="s">
-        <v>92</v>
-      </c>
+      <c r="V13" s="9"/>
+      <c r="W13" s="54"/>
       <c r="X13" s="54"/>
       <c r="Y13" s="54"/>
       <c r="Z13" s="54"/>
@@ -11553,41 +11353,25 @@
         <v>Fatigue_STRESS</v>
       </c>
       <c r="C14" s="35"/>
-      <c r="D14" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="100">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="126" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="35">
-        <v>8</v>
-      </c>
+      <c r="D14" s="110"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="35"/>
       <c r="I14" s="35"/>
       <c r="J14" s="35"/>
       <c r="K14" s="35"/>
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="34"/>
-      <c r="O14" s="110" t="s">
-        <v>78</v>
-      </c>
+      <c r="O14" s="110"/>
       <c r="P14" s="35"/>
       <c r="Q14" s="35"/>
       <c r="R14" s="35"/>
       <c r="S14" s="35"/>
       <c r="T14" s="35"/>
       <c r="U14" s="34"/>
-      <c r="V14" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="V14" s="9"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
       <c r="Y14" s="54"/>
@@ -11605,41 +11389,25 @@
         <v/>
       </c>
       <c r="C15" s="35"/>
-      <c r="D15" s="110">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="100">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" s="126" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" s="35">
-        <v>3</v>
-      </c>
+      <c r="D15" s="110"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="126"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
       <c r="K15" s="35"/>
       <c r="L15" s="35"/>
       <c r="M15" s="35"/>
       <c r="N15" s="34"/>
-      <c r="O15" s="110" t="s">
-        <v>74</v>
-      </c>
+      <c r="O15" s="110"/>
       <c r="P15" s="35"/>
       <c r="Q15" s="35"/>
       <c r="R15" s="35"/>
       <c r="S15" s="35"/>
       <c r="T15" s="35"/>
       <c r="U15" s="34"/>
-      <c r="V15" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="V15" s="9"/>
       <c r="W15" s="54"/>
       <c r="X15" s="54"/>
       <c r="Y15" s="54"/>
@@ -11657,14 +11425,8 @@
         <v/>
       </c>
       <c r="C16" s="35"/>
-      <c r="D16" s="110" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E16" s="100" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="D16" s="110"/>
+      <c r="E16" s="100"/>
       <c r="F16" s="35"/>
       <c r="G16" s="34"/>
       <c r="H16" s="35"/>
@@ -11700,11 +11462,11 @@
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="110" t="str">
+        <f t="shared" ref="D5:D40" si="1">IF(E17="","",0)</f>
+        <v/>
+      </c>
+      <c r="E17" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E17" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F17" s="54"/>
@@ -11741,11 +11503,11 @@
         <v/>
       </c>
       <c r="D18" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E18" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E18" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F18" s="54"/>
@@ -11782,11 +11544,11 @@
         <v/>
       </c>
       <c r="D19" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E19" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E19" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F19" s="54"/>
@@ -11823,11 +11585,11 @@
         <v/>
       </c>
       <c r="D20" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E20" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E20" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F20" s="54"/>
@@ -11865,11 +11627,11 @@
       </c>
       <c r="C21" s="125"/>
       <c r="D21" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E21" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E21" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F21" s="54"/>
@@ -11906,11 +11668,11 @@
         <v/>
       </c>
       <c r="D22" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E22" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E22" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F22" s="54"/>
@@ -11939,11 +11701,11 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D23" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E23" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E23" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F23" s="54"/>
@@ -11972,11 +11734,11 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D24" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E24" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E24" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F24" s="54"/>
@@ -12005,11 +11767,11 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D25" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E25" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E25" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F25" s="54"/>
@@ -12038,11 +11800,11 @@
     </row>
     <row r="26" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D26" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E26" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E26" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F26" s="54"/>
@@ -12070,16 +11832,16 @@
       <c r="AB26" s="5"/>
     </row>
     <row r="27" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="188" t="s">
-        <v>229</v>
-      </c>
-      <c r="B27" s="189"/>
+      <c r="A27" s="189" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27" s="190"/>
       <c r="D27" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E27" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E27" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F27" s="54"/>
@@ -12111,14 +11873,14 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D28" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E28" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E28" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F28" s="54"/>
@@ -12153,11 +11915,11 @@
         <v>81</v>
       </c>
       <c r="D29" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E29" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E29" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F29" s="54"/>
@@ -12192,11 +11954,11 @@
         <v>86</v>
       </c>
       <c r="D30" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E30" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E30" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F30" s="54"/>
@@ -12228,14 +11990,14 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D31" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E31" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E31" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F31" s="54"/>
@@ -12267,14 +12029,14 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D32" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E32" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E32" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F32" s="54"/>
@@ -12309,11 +12071,11 @@
         <v>83</v>
       </c>
       <c r="D33" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E33" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E33" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F33" s="54"/>
@@ -12345,14 +12107,14 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D34" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E34" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E34" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F34" s="54"/>
@@ -12384,14 +12146,14 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D35" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E35" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E35" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F35" s="54"/>
@@ -12423,14 +12185,14 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D36" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E36" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E36" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F36" s="54"/>
@@ -12462,14 +12224,14 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E37" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E37" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F37" s="54"/>
@@ -12501,14 +12263,14 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D38" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E38" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E38" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F38" s="54"/>
@@ -12540,14 +12302,14 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D39" s="110" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E39" s="100" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E39" s="100" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F39" s="54"/>
@@ -12579,14 +12341,14 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D40" s="111" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E40" s="176" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E40" s="176" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F40" s="7"/>
@@ -12618,7 +12380,7 @@
         <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
@@ -12672,7 +12434,7 @@
   <dimension ref="A1:XFD105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12709,83 +12471,83 @@
     <row r="1" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="105" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E2" s="106" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F2" s="106" t="s">
         <v>64</v>
       </c>
       <c r="G2" s="107" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="106" t="s">
+        <v>221</v>
+      </c>
+      <c r="I2" s="106" t="s">
+        <v>222</v>
+      </c>
+      <c r="J2" s="106" t="s">
+        <v>223</v>
+      </c>
+      <c r="K2" s="106" t="s">
+        <v>224</v>
+      </c>
+      <c r="L2" s="106" t="s">
+        <v>225</v>
+      </c>
+      <c r="M2" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="N2" s="106" t="s">
+        <v>227</v>
+      </c>
+      <c r="O2" s="106" t="s">
         <v>228</v>
       </c>
-      <c r="H2" s="106" t="s">
+      <c r="P2" s="106" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q2" s="106" t="s">
         <v>230</v>
       </c>
-      <c r="I2" s="106" t="s">
+      <c r="R2" s="106" t="s">
         <v>231</v>
       </c>
-      <c r="J2" s="106" t="s">
+      <c r="S2" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="K2" s="106" t="s">
+      <c r="T2" s="106" t="s">
         <v>233</v>
       </c>
-      <c r="L2" s="106" t="s">
+      <c r="U2" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="M2" s="106" t="s">
+      <c r="V2" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="N2" s="106" t="s">
+      <c r="W2" s="106" t="s">
         <v>236</v>
       </c>
-      <c r="O2" s="106" t="s">
+      <c r="X2" s="106" t="s">
         <v>237</v>
       </c>
-      <c r="P2" s="106" t="s">
+      <c r="Y2" s="106" t="s">
         <v>238</v>
       </c>
-      <c r="Q2" s="106" t="s">
+      <c r="Z2" s="107" t="s">
         <v>239</v>
       </c>
-      <c r="R2" s="106" t="s">
+      <c r="AA2" s="106" t="s">
         <v>240</v>
-      </c>
-      <c r="S2" s="106" t="s">
-        <v>241</v>
-      </c>
-      <c r="T2" s="106" t="s">
-        <v>242</v>
-      </c>
-      <c r="U2" s="106" t="s">
-        <v>243</v>
-      </c>
-      <c r="V2" s="106" t="s">
-        <v>244</v>
-      </c>
-      <c r="W2" s="106" t="s">
-        <v>245</v>
-      </c>
-      <c r="X2" s="106" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y2" s="106" t="s">
-        <v>247</v>
-      </c>
-      <c r="Z2" s="107" t="s">
-        <v>248</v>
-      </c>
-      <c r="AA2" s="106" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
@@ -12799,29 +12561,25 @@
       </c>
       <c r="C3" s="35"/>
       <c r="D3" s="110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="108">
         <v>1</v>
       </c>
       <c r="F3" s="108" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="H3" s="100" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="I3" s="34">
-        <v>4</v>
-      </c>
-      <c r="J3" s="100" t="s">
-        <v>285</v>
-      </c>
-      <c r="K3" s="54">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J3" s="100"/>
+      <c r="K3" s="54"/>
       <c r="L3" s="3"/>
       <c r="M3" s="5"/>
       <c r="N3" s="3"/>
@@ -12850,7 +12608,7 @@
       </c>
       <c r="C4" s="35"/>
       <c r="D4" s="110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="108">
         <f>IF(G4="","",E3+1)</f>
@@ -12860,20 +12618,16 @@
         <v>86</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="H4" s="112" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="I4" s="34">
-        <v>4</v>
-      </c>
-      <c r="J4" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="K4" s="34">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J4" s="112"/>
+      <c r="K4" s="34"/>
       <c r="L4" s="3"/>
       <c r="M4" s="5"/>
       <c r="N4" s="3"/>
@@ -12906,30 +12660,26 @@
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="108">
         <f t="shared" ref="E5" si="0">IF(G5="","",E4+1)</f>
         <v>3</v>
       </c>
       <c r="F5" s="108" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="H5" s="112" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="I5" s="34">
-        <v>4</v>
-      </c>
-      <c r="J5" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="K5" s="34">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J5" s="112"/>
+      <c r="K5" s="34"/>
       <c r="L5" s="3"/>
       <c r="M5" s="5"/>
       <c r="N5" s="3"/>
@@ -15782,35 +15532,35 @@
     <row r="1" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="121"/>
       <c r="D2" s="106" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="106" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="105" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="106" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="120" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="106" t="s">
         <v>157</v>
       </c>
-      <c r="E2" s="106" t="s">
-        <v>272</v>
-      </c>
-      <c r="F2" s="105" t="s">
+      <c r="J2" s="120" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="106" t="s">
+      <c r="K2" s="106" t="s">
         <v>159</v>
-      </c>
-      <c r="H2" s="120" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="106" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="120" t="s">
-        <v>162</v>
-      </c>
-      <c r="K2" s="106" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
@@ -15830,7 +15580,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G3" s="123">
         <v>1</v>
@@ -15865,7 +15615,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G4" s="20">
         <v>1</v>
@@ -15883,7 +15633,7 @@
         <v>3</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
@@ -15915,7 +15665,7 @@
       <c r="J5" s="54"/>
       <c r="K5" s="5"/>
       <c r="AL5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="AS5" s="9" t="s">
         <v>92</v>
@@ -16483,7 +16233,7 @@
         <v>46</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>72</v>
@@ -16492,37 +16242,37 @@
         <v>73</v>
       </c>
       <c r="M2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="P2" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="Q2" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="O2" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>149</v>
-      </c>
       <c r="R2" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="S2" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="U2" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="U2" s="21" t="s">
-        <v>103</v>
-      </c>
       <c r="V2" s="21" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="W2" s="21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -16577,7 +16327,7 @@
         <v>48</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
@@ -16597,7 +16347,7 @@
         <v>51</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.3">
@@ -16613,7 +16363,7 @@
         <v>53</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
@@ -16632,14 +16382,14 @@
       <c r="B14" s="20"/>
     </row>
     <row r="15" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="187" t="s">
+      <c r="B15" s="188" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="185"/>
-      <c r="D15" s="185"/>
-      <c r="E15" s="185"/>
-      <c r="F15" s="185"/>
-      <c r="G15" s="186"/>
+      <c r="C15" s="186"/>
+      <c r="D15" s="186"/>
+      <c r="E15" s="186"/>
+      <c r="F15" s="186"/>
+      <c r="G15" s="187"/>
     </row>
     <row r="16" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="105" t="s">
@@ -16663,22 +16413,22 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="32" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -16887,16 +16637,16 @@
   <sheetData>
     <row r="1" spans="2:33" s="28" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C1" s="74" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E1" s="74" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G1" s="73" t="s">
         <v>32</v>
@@ -16915,19 +16665,19 @@
         <v>69</v>
       </c>
       <c r="M1" s="74" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N1" s="75" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P1" s="57" t="s">
         <v>71</v>
       </c>
       <c r="Q1" s="58" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="R1" s="51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S1" s="71" t="s">
         <v>66</v>
@@ -16936,22 +16686,22 @@
         <v>67</v>
       </c>
       <c r="U1" s="58" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="V1" s="51" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="W1" s="58" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="X1" s="51" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="Y1" s="58" t="s">
         <v>70</v>
       </c>
       <c r="Z1" s="51" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AA1" s="58" t="s">
         <v>17</v>
@@ -16966,13 +16716,13 @@
         <v>76</v>
       </c>
       <c r="AE1" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AF1" s="43" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AG1" s="43" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="2:33" x14ac:dyDescent="0.3">
@@ -16995,7 +16745,7 @@
         <v>1.383</v>
       </c>
       <c r="I2" s="83" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J2" s="80" t="s">
         <v>63</v>
@@ -17020,10 +16770,10 @@
         <v>0.5</v>
       </c>
       <c r="S2" s="59" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T2" s="89" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U2" s="89">
         <v>0.5</v>
@@ -17086,10 +16836,10 @@
         <v>3</v>
       </c>
       <c r="I3" s="84" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J3" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K3" s="54"/>
       <c r="L3" s="78">
@@ -17112,10 +16862,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="S3" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T3" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U3" s="90">
         <v>0.5</v>
@@ -17168,10 +16918,10 @@
         <v>1.27</v>
       </c>
       <c r="I4" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J4" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K4" s="54"/>
       <c r="L4" s="78">
@@ -17194,10 +16944,10 @@
         <v>2</v>
       </c>
       <c r="S4" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T4" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U4" s="90">
         <v>0.5</v>
@@ -17250,10 +17000,10 @@
         <v>1.27</v>
       </c>
       <c r="I5" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J5" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K5" s="54"/>
       <c r="L5" s="78">
@@ -17276,10 +17026,10 @@
         <v>3.5</v>
       </c>
       <c r="S5" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T5" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U5" s="90">
         <v>0.5</v>
@@ -17332,7 +17082,7 @@
         <v>1.325</v>
       </c>
       <c r="I6" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J6" s="81" t="s">
         <v>63</v>
@@ -17358,10 +17108,10 @@
         <v>4</v>
       </c>
       <c r="S6" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T6" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U6" s="90">
         <v>0.5</v>
@@ -17414,10 +17164,10 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="I7" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J7" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K7" s="54"/>
       <c r="L7" s="78">
@@ -17440,10 +17190,10 @@
         <v>5</v>
       </c>
       <c r="S7" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T7" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U7" s="90">
         <v>0.5</v>
@@ -17496,10 +17246,10 @@
         <v>1.23</v>
       </c>
       <c r="I8" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J8" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K8" s="54"/>
       <c r="L8" s="78">
@@ -17522,10 +17272,10 @@
         <v>5.9</v>
       </c>
       <c r="S8" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T8" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U8" s="90">
         <v>0.5</v>
@@ -17578,10 +17328,10 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="I9" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J9" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K9" s="54"/>
       <c r="L9" s="78">
@@ -17604,10 +17354,10 @@
         <v>10.9</v>
       </c>
       <c r="S9" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T9" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U9" s="90">
         <v>0.5</v>
@@ -17660,10 +17410,10 @@
         <v>1.23</v>
       </c>
       <c r="I10" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J10" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K10" s="54"/>
       <c r="L10" s="78">
@@ -17686,10 +17436,10 @@
         <v>14</v>
       </c>
       <c r="S10" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T10" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U10" s="90">
         <v>0.5</v>
@@ -17742,10 +17492,10 @@
         <v>1.23</v>
       </c>
       <c r="I11" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J11" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K11" s="54"/>
       <c r="L11" s="78">
@@ -17768,10 +17518,10 @@
         <v>16.5</v>
       </c>
       <c r="S11" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T11" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U11" s="90">
         <v>0.5</v>
@@ -17824,10 +17574,10 @@
         <v>1.23</v>
       </c>
       <c r="I12" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J12" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K12" s="54"/>
       <c r="L12" s="78">
@@ -17850,10 +17600,10 @@
         <v>19.8</v>
       </c>
       <c r="S12" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T12" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U12" s="90">
         <v>0.5</v>
@@ -17906,10 +17656,10 @@
         <v>3</v>
       </c>
       <c r="I13" s="84" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J13" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K13" s="54"/>
       <c r="L13" s="78">
@@ -17932,10 +17682,10 @@
         <v>30</v>
       </c>
       <c r="S13" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T13" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U13" s="90">
         <v>0.5</v>
@@ -17988,10 +17738,10 @@
         <v>3</v>
       </c>
       <c r="I14" s="84" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J14" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K14" s="54"/>
       <c r="L14" s="79">
@@ -18015,10 +17765,10 @@
         <v>42.8</v>
       </c>
       <c r="S14" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T14" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U14" s="90">
         <v>0.5</v>
@@ -18071,10 +17821,10 @@
         <v>1.07</v>
       </c>
       <c r="I15" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J15" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K15" s="54"/>
       <c r="P15" s="60">
@@ -18088,10 +17838,10 @@
         <v>47.5</v>
       </c>
       <c r="S15" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T15" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U15" s="90">
         <v>0.5</v>
@@ -18144,10 +17894,10 @@
         <v>1.07</v>
       </c>
       <c r="I16" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J16" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K16" s="54"/>
       <c r="P16" s="60">
@@ -18161,10 +17911,10 @@
         <v>55</v>
       </c>
       <c r="S16" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T16" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U16" s="90">
         <v>0.5</v>
@@ -18216,10 +17966,10 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="I17" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J17" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K17" s="54"/>
       <c r="P17" s="60">
@@ -18233,10 +17983,10 @@
         <v>61</v>
       </c>
       <c r="S17" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T17" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U17" s="90">
         <v>0.5</v>
@@ -18288,10 +18038,10 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="I18" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J18" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K18" s="54"/>
       <c r="P18" s="61">
@@ -18305,10 +18055,10 @@
         <v>80</v>
       </c>
       <c r="S18" s="60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T18" s="90" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U18" s="90">
         <v>0.5</v>
@@ -18360,10 +18110,10 @@
         <v>3</v>
       </c>
       <c r="I19" s="84" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J19" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K19" s="54"/>
       <c r="P19" s="60"/>
@@ -18397,7 +18147,7 @@
         <v>1.0509999999999999</v>
       </c>
       <c r="I20" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J20" s="81" t="s">
         <v>63</v>
@@ -18434,10 +18184,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="I21" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J21" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K21" s="54"/>
       <c r="P21" s="60"/>
@@ -18471,10 +18221,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="I22" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J22" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K22" s="54"/>
       <c r="P22" s="60"/>
@@ -18508,7 +18258,7 @@
         <v>0.97599999999999998</v>
       </c>
       <c r="I23" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J23" s="81" t="s">
         <v>63</v>
@@ -18545,7 +18295,7 @@
         <v>1.0509999999999999</v>
       </c>
       <c r="I24" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J24" s="81" t="s">
         <v>63</v>
@@ -18582,10 +18332,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I25" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J25" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K25" s="54"/>
       <c r="P25" s="60"/>
@@ -18619,10 +18369,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I26" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J26" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K26" s="54"/>
       <c r="P26" s="60"/>
@@ -18656,7 +18406,7 @@
         <v>1.524</v>
       </c>
       <c r="I27" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J27" s="81" t="s">
         <v>63</v>
@@ -18693,10 +18443,10 @@
         <v>2</v>
       </c>
       <c r="I28" s="84" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J28" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K28" s="54"/>
       <c r="P28" s="60"/>
@@ -18731,7 +18481,7 @@
         <v>1.145</v>
       </c>
       <c r="I29" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J29" s="81" t="s">
         <v>63</v>
@@ -18769,10 +18519,10 @@
         <v>1.4</v>
       </c>
       <c r="I30" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J30" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K30" s="54"/>
       <c r="P30" s="60"/>
@@ -18807,10 +18557,10 @@
         <v>1.4</v>
       </c>
       <c r="I31" s="84" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J31" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K31" s="54"/>
       <c r="P31" s="60"/>
@@ -18845,7 +18595,7 @@
         <v>1.143</v>
       </c>
       <c r="I32" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J32" s="81" t="s">
         <v>63</v>
@@ -18883,7 +18633,7 @@
         <v>1.048</v>
       </c>
       <c r="I33" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J33" s="81" t="s">
         <v>63</v>
@@ -18921,7 +18671,7 @@
         <v>1.18</v>
       </c>
       <c r="I34" s="84" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J34" s="81" t="s">
         <v>63</v>
@@ -19793,16 +19543,16 @@
   <sheetData>
     <row r="1" spans="2:33" s="167" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="171" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C1" s="170" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D1" s="170" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E1" s="172" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G1" s="171" t="s">
         <v>32</v>
@@ -19820,19 +19570,19 @@
         <v>69</v>
       </c>
       <c r="M1" s="172" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N1" s="172" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P1" s="171" t="s">
         <v>71</v>
       </c>
       <c r="Q1" s="170" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="R1" s="170" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="S1" s="170" t="s">
         <v>66</v>
@@ -19841,22 +19591,22 @@
         <v>67</v>
       </c>
       <c r="U1" s="170" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="V1" s="170" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="W1" s="170" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="X1" s="170" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="Y1" s="170" t="s">
         <v>70</v>
       </c>
       <c r="Z1" s="170" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AA1" s="170" t="s">
         <v>17</v>
@@ -19871,13 +19621,13 @@
         <v>76</v>
       </c>
       <c r="AE1" s="169" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AF1" s="169" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AG1" s="168" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="2:33" x14ac:dyDescent="0.3">
@@ -19900,7 +19650,7 @@
         <v>1.383</v>
       </c>
       <c r="I2" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J2" s="154" t="s">
         <v>63</v>
@@ -19924,10 +19674,10 @@
         <v>1.7</v>
       </c>
       <c r="S2" s="158" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T2" s="174" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U2" s="163">
         <v>0.5</v>
@@ -19989,10 +19739,10 @@
         <v>3</v>
       </c>
       <c r="I3" s="155" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J3" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L3" s="156">
         <v>2</v>
@@ -20014,10 +19764,10 @@
         <v>2.5</v>
       </c>
       <c r="S3" s="158" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="T3" s="174" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="U3" s="157">
         <v>0.5</v>
@@ -20065,10 +19815,10 @@
         <v>1.27</v>
       </c>
       <c r="I4" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J4" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L4" s="156">
         <v>3</v>
@@ -20090,10 +19840,10 @@
         <v>4</v>
       </c>
       <c r="S4" s="158" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T4" s="174" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U4" s="157">
         <v>0.5</v>
@@ -20141,10 +19891,10 @@
         <v>1.27</v>
       </c>
       <c r="I5" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J5" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L5" s="156">
         <v>4</v>
@@ -20166,10 +19916,10 @@
         <v>5.5</v>
       </c>
       <c r="S5" s="158" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T5" s="174" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U5" s="157">
         <v>0.5</v>
@@ -20217,7 +19967,7 @@
         <v>1.325</v>
       </c>
       <c r="I6" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J6" s="154" t="s">
         <v>63</v>
@@ -20242,10 +19992,10 @@
         <v>9</v>
       </c>
       <c r="S6" s="158" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="T6" s="174" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="U6" s="157">
         <v>0.5</v>
@@ -20293,10 +20043,10 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="I7" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J7" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L7" s="156">
         <v>6</v>
@@ -20318,10 +20068,10 @@
         <v>14</v>
       </c>
       <c r="S7" s="158" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T7" s="174" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U7" s="157">
         <v>0.5</v>
@@ -20369,10 +20119,10 @@
         <v>1.23</v>
       </c>
       <c r="I8" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J8" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L8" s="156">
         <v>7</v>
@@ -20394,10 +20144,10 @@
         <v>25</v>
       </c>
       <c r="S8" s="158" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="T8" s="174" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="U8" s="157">
         <v>0.5</v>
@@ -20445,10 +20195,10 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="I9" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J9" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L9" s="156">
         <v>8</v>
@@ -20470,10 +20220,10 @@
         <v>40.299999999999997</v>
       </c>
       <c r="S9" s="158" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="T9" s="174" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="U9" s="157">
         <v>0.5</v>
@@ -20522,10 +20272,10 @@
         <v>1.23</v>
       </c>
       <c r="I10" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J10" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L10" s="156">
         <v>9</v>
@@ -20547,10 +20297,10 @@
         <v>43.8</v>
       </c>
       <c r="S10" s="158" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="T10" s="174" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U10" s="157">
         <v>0.5</v>
@@ -20599,10 +20349,10 @@
         <v>1.23</v>
       </c>
       <c r="I11" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J11" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L11" s="156">
         <v>10</v>
@@ -20624,10 +20374,10 @@
         <v>95</v>
       </c>
       <c r="S11" s="158" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="T11" s="174" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="U11" s="157">
         <v>0.5</v>
@@ -20678,10 +20428,10 @@
         <v>1.23</v>
       </c>
       <c r="I12" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J12" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L12" s="156">
         <v>11</v>
@@ -20704,10 +20454,10 @@
         <v>3</v>
       </c>
       <c r="I13" s="155" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J13" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L13" s="156">
         <v>12</v>
@@ -20730,10 +20480,10 @@
         <v>3</v>
       </c>
       <c r="I14" s="155" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J14" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L14" s="161">
         <v>13</v>
@@ -20756,10 +20506,10 @@
         <v>1.07</v>
       </c>
       <c r="I15" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J15" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P15" s="3"/>
       <c r="AE15" s="5"/>
@@ -20772,10 +20522,10 @@
         <v>1.07</v>
       </c>
       <c r="I16" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J16" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P16" s="3"/>
       <c r="AE16" s="5"/>
@@ -20788,10 +20538,10 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="I17" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J17" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P17" s="3"/>
       <c r="AE17" s="5"/>
@@ -20804,10 +20554,10 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="I18" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J18" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P18" s="3"/>
       <c r="AE18" s="5"/>
@@ -20820,10 +20570,10 @@
         <v>3</v>
       </c>
       <c r="I19" s="155" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J19" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P19" s="3"/>
       <c r="AE19" s="5"/>
@@ -20836,7 +20586,7 @@
         <v>1.0509999999999999</v>
       </c>
       <c r="I20" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J20" s="154" t="s">
         <v>63</v>
@@ -20852,10 +20602,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="I21" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J21" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P21" s="3"/>
       <c r="AE21" s="5"/>
@@ -20868,10 +20618,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="I22" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J22" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P22" s="3"/>
       <c r="AE22" s="5"/>
@@ -20884,7 +20634,7 @@
         <v>0.97599999999999998</v>
       </c>
       <c r="I23" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J23" s="154" t="s">
         <v>63</v>
@@ -20900,7 +20650,7 @@
         <v>1.0509999999999999</v>
       </c>
       <c r="I24" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J24" s="154" t="s">
         <v>63</v>
@@ -20916,10 +20666,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I25" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J25" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P25" s="3"/>
       <c r="AE25" s="5"/>
@@ -20932,10 +20682,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I26" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J26" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P26" s="3"/>
       <c r="AE26" s="5"/>
@@ -20948,7 +20698,7 @@
         <v>1.524</v>
       </c>
       <c r="I27" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J27" s="154" t="s">
         <v>63</v>
@@ -20964,10 +20714,10 @@
         <v>2</v>
       </c>
       <c r="I28" s="155" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J28" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P28" s="3"/>
       <c r="AE28" s="5"/>
@@ -20981,7 +20731,7 @@
         <v>1.145</v>
       </c>
       <c r="I29" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J29" s="154" t="s">
         <v>63</v>
@@ -20998,10 +20748,10 @@
         <v>1.4</v>
       </c>
       <c r="I30" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J30" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P30" s="3"/>
       <c r="AE30" s="5"/>
@@ -21018,10 +20768,10 @@
         <v>1.4</v>
       </c>
       <c r="I31" s="155" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J31" s="154" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P31" s="3"/>
       <c r="AE31" s="5"/>
@@ -21038,7 +20788,7 @@
         <v>1.143</v>
       </c>
       <c r="I32" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J32" s="154" t="s">
         <v>63</v>
@@ -21058,7 +20808,7 @@
         <v>1.048</v>
       </c>
       <c r="I33" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J33" s="154" t="s">
         <v>63</v>
@@ -21078,7 +20828,7 @@
         <v>1.18</v>
       </c>
       <c r="I34" s="155" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J34" s="154" t="s">
         <v>63</v>
@@ -21267,7 +21017,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="153" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J61" s="5"/>
     </row>
@@ -21279,38 +21029,38 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="153" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="J63" s="5"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="153" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="153" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="153" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="153" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="153" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="153" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -21368,13 +21118,13 @@
     <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="116" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C2" s="116" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D2" s="116" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -21382,18 +21132,18 @@
         <v>41</v>
       </c>
       <c r="C3" s="114" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D3" s="114" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="114" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C4" s="114" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D4" s="114" t="s">
         <v>86</v>
@@ -21404,27 +21154,27 @@
         <v>68</v>
       </c>
       <c r="C5" s="114" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D5" s="114" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="114" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C6" s="114" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D6" s="114"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="114" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C7" s="114" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D7" s="114"/>
     </row>

</xml_diff>

<commit_message>
Merge of excel input with hybrid pile
</commit_message>
<xml_diff>
--- a/Input/PDAcalc.xlsx
+++ b/Input/PDAcalc.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ADD6D0-A5AC-4453-8127-8AF5360C0BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91C22E5-CBF7-4844-831A-F007E664DA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="652" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="1416" windowWidth="23256" windowHeight="12576" tabRatio="652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCATIONS" sheetId="66" r:id="rId1"/>
@@ -386,6 +386,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="AB25" authorId="0" shapeId="0" xr:uid="{2A9C6DEB-CD8F-4919-AF0A-E8E7B095418B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+0 = normal driving
+1 = hybrid driving, depth is distance from embedment depth
+2 = hybrid driving, depth is distance from mudline</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A31" authorId="0" shapeId="0" xr:uid="{576C90F1-D1EC-4115-B2DF-9179E2FEAB98}">
       <text>
         <r>
@@ -744,7 +770,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="299">
   <si>
     <t>Setting</t>
   </si>
@@ -1635,13 +1661,22 @@
   </si>
   <si>
     <t>Lehane</t>
+  </si>
+  <si>
+    <t>Hybrid pile</t>
+  </si>
+  <si>
+    <t>Hybrid driving strategy</t>
+  </si>
+  <si>
+    <t>Depth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1722,6 +1757,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2430,7 +2478,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2760,45 +2808,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2825,6 +2834,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2833,18 +2884,7 @@
     <cellStyle name="Normal 3" xfId="3" xr:uid="{BB2A21B6-ED26-4A17-A481-3F1C823DC031}"/>
     <cellStyle name="Normal 4" xfId="4" xr:uid="{DC5E9318-48F4-4F4E-B624-85906B79C1B1}"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <font>
         <b val="0"/>
@@ -8262,12 +8302,12 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="31" priority="2">
+    <cfRule type="expression" dxfId="30" priority="2">
       <formula>$D2=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:W1048576">
-    <cfRule type="expression" dxfId="30" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>$A2=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8289,8 +8329,8 @@
   </sheetPr>
   <dimension ref="A1:AB81"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8342,15 +8382,15 @@
       <c r="I2" s="148" t="s">
         <v>171</v>
       </c>
-      <c r="K2" s="179" t="s">
+      <c r="K2" s="201" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="180"/>
+      <c r="L2" s="202"/>
       <c r="M2" s="53"/>
-      <c r="N2" s="179" t="s">
+      <c r="N2" s="201" t="s">
         <v>226</v>
       </c>
-      <c r="O2" s="180"/>
+      <c r="O2" s="202"/>
     </row>
     <row r="3" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13">
@@ -8827,10 +8867,10 @@
       <c r="G16" s="54"/>
       <c r="H16" s="54"/>
       <c r="I16" s="34"/>
-      <c r="K16" s="179" t="s">
+      <c r="K16" s="201" t="s">
         <v>216</v>
       </c>
-      <c r="L16" s="180"/>
+      <c r="L16" s="202"/>
     </row>
     <row r="17" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
@@ -8949,36 +8989,36 @@
       <c r="N22" s="53"/>
       <c r="O22" s="53"/>
     </row>
-    <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="177" t="s">
+      <c r="B24" s="199" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="184"/>
-      <c r="D24" s="184"/>
-      <c r="E24" s="184"/>
-      <c r="F24" s="184"/>
-      <c r="G24" s="184"/>
-      <c r="H24" s="184"/>
-      <c r="I24" s="184"/>
-      <c r="J24" s="184"/>
-      <c r="K24" s="184"/>
-      <c r="L24" s="184"/>
-      <c r="M24" s="184"/>
-      <c r="N24" s="184"/>
-      <c r="O24" s="184"/>
-      <c r="P24" s="184"/>
-      <c r="Q24" s="184"/>
-      <c r="R24" s="184"/>
-      <c r="S24" s="184"/>
-      <c r="T24" s="184"/>
-      <c r="U24" s="184"/>
-      <c r="V24" s="184"/>
-      <c r="W24" s="184"/>
-      <c r="X24" s="184"/>
-      <c r="Y24" s="184"/>
-      <c r="Z24" s="184"/>
-      <c r="AA24" s="178"/>
+      <c r="C24" s="200"/>
+      <c r="D24" s="200"/>
+      <c r="E24" s="200"/>
+      <c r="F24" s="200"/>
+      <c r="G24" s="200"/>
+      <c r="H24" s="200"/>
+      <c r="I24" s="200"/>
+      <c r="J24" s="200"/>
+      <c r="K24" s="200"/>
+      <c r="L24" s="200"/>
+      <c r="M24" s="200"/>
+      <c r="N24" s="200"/>
+      <c r="O24" s="200"/>
+      <c r="P24" s="200"/>
+      <c r="Q24" s="200"/>
+      <c r="R24" s="200"/>
+      <c r="S24" s="200"/>
+      <c r="T24" s="200"/>
+      <c r="U24" s="200"/>
+      <c r="V24" s="200"/>
+      <c r="W24" s="200"/>
+      <c r="X24" s="200"/>
+      <c r="Y24" s="200"/>
+      <c r="Z24" s="200"/>
+      <c r="AA24" s="200"/>
+      <c r="AB24" s="200"/>
     </row>
     <row r="25" spans="1:28" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="150" t="s">
@@ -9059,7 +9099,9 @@
       <c r="AA25" s="152" t="s">
         <v>152</v>
       </c>
-      <c r="AB25" s="53"/>
+      <c r="AB25" s="145" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="52"/>
@@ -9137,6 +9179,9 @@
         <v>0</v>
       </c>
       <c r="AA26" s="155">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="156">
         <v>0</v>
       </c>
     </row>
@@ -9219,6 +9264,9 @@
       <c r="AA27" s="156">
         <v>0</v>
       </c>
+      <c r="AB27" s="156">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="52"/>
@@ -9299,6 +9347,9 @@
       <c r="AA28" s="156">
         <v>0</v>
       </c>
+      <c r="AB28" s="156">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="52"/>
@@ -9379,6 +9430,9 @@
       <c r="AA29" s="156">
         <v>0</v>
       </c>
+      <c r="AB29" s="156">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="52"/>
@@ -9459,6 +9513,9 @@
       <c r="AA30" s="156">
         <v>0</v>
       </c>
+      <c r="AB30" s="156">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="52"/>
@@ -9539,6 +9596,9 @@
       <c r="AA31" s="156">
         <v>0</v>
       </c>
+      <c r="AB31" s="156">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="52"/>
@@ -9619,8 +9679,11 @@
       <c r="AA32" s="156">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB32" s="156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="52"/>
       <c r="B33" s="52">
         <f t="shared" si="3"/>
@@ -9699,8 +9762,11 @@
       <c r="AA33" s="156">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB33" s="156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="52"/>
       <c r="B34" s="52">
         <f t="shared" si="3"/>
@@ -9779,8 +9845,11 @@
       <c r="AA34" s="156">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB34" s="156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="52"/>
       <c r="B35" s="52">
         <f t="shared" si="3"/>
@@ -9859,8 +9928,11 @@
       <c r="AA35" s="156">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB35" s="156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
       <c r="B36" s="52">
         <f t="shared" si="3"/>
@@ -9939,8 +10011,11 @@
       <c r="AA36" s="156">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB36" s="156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="52"/>
       <c r="B37" s="52">
         <f t="shared" si="3"/>
@@ -10019,8 +10094,11 @@
       <c r="AA37" s="156">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:27" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB37" s="156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="142"/>
       <c r="B38" s="52" t="str">
         <f t="shared" si="3"/>
@@ -10051,8 +10129,9 @@
       <c r="Y38" s="142"/>
       <c r="Z38" s="142"/>
       <c r="AA38" s="156"/>
-    </row>
-    <row r="39" spans="1:27" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB38" s="156"/>
+    </row>
+    <row r="39" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
       <c r="B39" s="52" t="str">
         <f t="shared" si="3"/>
@@ -10083,8 +10162,9 @@
       <c r="Y39" s="142"/>
       <c r="Z39" s="142"/>
       <c r="AA39" s="156"/>
-    </row>
-    <row r="40" spans="1:27" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB39" s="156"/>
+    </row>
+    <row r="40" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="52"/>
       <c r="B40" s="52" t="str">
         <f t="shared" si="3"/>
@@ -10115,8 +10195,9 @@
       <c r="Y40" s="142"/>
       <c r="Z40" s="142"/>
       <c r="AA40" s="156"/>
-    </row>
-    <row r="41" spans="1:27" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB40" s="156"/>
+    </row>
+    <row r="41" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="52"/>
       <c r="B41" s="52" t="str">
         <f t="shared" si="3"/>
@@ -10147,8 +10228,9 @@
       <c r="Y41" s="142"/>
       <c r="Z41" s="142"/>
       <c r="AA41" s="156"/>
-    </row>
-    <row r="42" spans="1:27" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB41" s="156"/>
+    </row>
+    <row r="42" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="52"/>
       <c r="B42" s="52" t="str">
         <f t="shared" si="3"/>
@@ -10179,8 +10261,9 @@
       <c r="Y42" s="142"/>
       <c r="Z42" s="142"/>
       <c r="AA42" s="156"/>
-    </row>
-    <row r="43" spans="1:27" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB42" s="156"/>
+    </row>
+    <row r="43" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="52"/>
       <c r="B43" s="52" t="str">
         <f t="shared" si="3"/>
@@ -10211,8 +10294,9 @@
       <c r="Y43" s="142"/>
       <c r="Z43" s="142"/>
       <c r="AA43" s="156"/>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB43" s="156"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="52"/>
       <c r="B44" s="52" t="str">
         <f t="shared" si="3"/>
@@ -10243,8 +10327,9 @@
       <c r="Y44" s="142"/>
       <c r="Z44" s="142"/>
       <c r="AA44" s="156"/>
-    </row>
-    <row r="45" spans="1:27" s="53" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB44" s="156"/>
+    </row>
+    <row r="45" spans="1:28" s="53" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="52"/>
       <c r="B45" s="55" t="str">
         <f t="shared" si="3"/>
@@ -10275,33 +10360,34 @@
       <c r="Y45" s="157"/>
       <c r="Z45" s="157"/>
       <c r="AA45" s="158"/>
-    </row>
-    <row r="46" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="181" t="s">
+      <c r="AB45" s="158"/>
+    </row>
+    <row r="46" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="191" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="182"/>
-      <c r="D47" s="182"/>
-      <c r="E47" s="182"/>
-      <c r="F47" s="182"/>
-      <c r="G47" s="182"/>
-      <c r="H47" s="183"/>
-      <c r="J47" s="181" t="s">
+      <c r="C47" s="192"/>
+      <c r="D47" s="192"/>
+      <c r="E47" s="192"/>
+      <c r="F47" s="192"/>
+      <c r="G47" s="192"/>
+      <c r="H47" s="193"/>
+      <c r="J47" s="191" t="s">
         <v>29</v>
       </c>
-      <c r="K47" s="182"/>
-      <c r="L47" s="182"/>
-      <c r="M47" s="182"/>
-      <c r="N47" s="182"/>
-      <c r="O47" s="182"/>
-      <c r="P47" s="182"/>
-      <c r="Q47" s="182"/>
-      <c r="R47" s="182"/>
-      <c r="S47" s="182"/>
-      <c r="T47" s="183"/>
-    </row>
-    <row r="48" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K47" s="192"/>
+      <c r="L47" s="192"/>
+      <c r="M47" s="192"/>
+      <c r="N47" s="192"/>
+      <c r="O47" s="192"/>
+      <c r="P47" s="192"/>
+      <c r="Q47" s="192"/>
+      <c r="R47" s="192"/>
+      <c r="S47" s="192"/>
+      <c r="T47" s="193"/>
+    </row>
+    <row r="48" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="143" t="s">
         <v>0</v>
       </c>
@@ -10657,10 +10743,14 @@
     </row>
     <row r="62" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="177" t="s">
+      <c r="B63" s="189" t="s">
         <v>131</v>
       </c>
-      <c r="C63" s="178"/>
+      <c r="C63" s="190"/>
+      <c r="E63" s="189" t="s">
+        <v>297</v>
+      </c>
+      <c r="F63" s="190"/>
     </row>
     <row r="64" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="143" t="s">
@@ -10669,124 +10759,173 @@
       <c r="C64" s="145" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E64" s="143" t="s">
+        <v>298</v>
+      </c>
+      <c r="F64" s="145" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="13">
         <v>1</v>
       </c>
       <c r="C65" s="2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E65" s="13">
+        <v>0</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="3">
         <v>2</v>
       </c>
       <c r="C66" s="5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E66" s="3">
+        <v>3</v>
+      </c>
+      <c r="F66" s="5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="3">
         <v>3</v>
       </c>
       <c r="C67" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E67" s="3"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="3">
         <v>4</v>
       </c>
       <c r="C68" s="5">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E68" s="3"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="3">
         <v>5</v>
       </c>
       <c r="C69" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E69" s="3"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="3">
         <v>6</v>
       </c>
       <c r="C70" s="5">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E70" s="3"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="3">
         <v>7</v>
       </c>
       <c r="C71" s="5">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E71" s="3"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="3">
         <v>8</v>
       </c>
       <c r="C72" s="5">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E72" s="3"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="3">
         <v>9</v>
       </c>
       <c r="C73" s="5">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E73" s="3"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="3">
         <v>10</v>
       </c>
       <c r="C74" s="5">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E74" s="3"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="3"/>
       <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E75" s="3"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="3"/>
       <c r="C76" s="5"/>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E76" s="3"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="3"/>
       <c r="C77" s="5"/>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E77" s="3"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
       <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E78" s="3"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="3"/>
       <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E79" s="3"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="3"/>
       <c r="C80" s="5"/>
-    </row>
-    <row r="81" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E80" s="3"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="6"/>
       <c r="C81" s="8"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="B47:H47"/>
     <mergeCell ref="J47:T47"/>
-    <mergeCell ref="B24:AA24"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="B24:AB24"/>
+    <mergeCell ref="E63:F63"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X27:X33 X37:X43" xr:uid="{3900C4C6-43F3-4DF6-8675-9B5D9868FF8C}">
@@ -10866,33 +11005,33 @@
       <c r="G2" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="185" t="s">
+      <c r="H2" s="194" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="185"/>
-      <c r="J2" s="185"/>
-      <c r="K2" s="185"/>
-      <c r="L2" s="185"/>
-      <c r="M2" s="185"/>
-      <c r="N2" s="186"/>
-      <c r="O2" s="187" t="s">
+      <c r="I2" s="194"/>
+      <c r="J2" s="194"/>
+      <c r="K2" s="194"/>
+      <c r="L2" s="194"/>
+      <c r="M2" s="194"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="196" t="s">
         <v>84</v>
       </c>
-      <c r="P2" s="185"/>
-      <c r="Q2" s="185"/>
-      <c r="R2" s="185"/>
-      <c r="S2" s="185"/>
-      <c r="T2" s="185"/>
-      <c r="U2" s="186"/>
-      <c r="V2" s="187" t="s">
+      <c r="P2" s="194"/>
+      <c r="Q2" s="194"/>
+      <c r="R2" s="194"/>
+      <c r="S2" s="194"/>
+      <c r="T2" s="194"/>
+      <c r="U2" s="195"/>
+      <c r="V2" s="196" t="s">
         <v>90</v>
       </c>
-      <c r="W2" s="185"/>
-      <c r="X2" s="185"/>
-      <c r="Y2" s="185"/>
-      <c r="Z2" s="185"/>
-      <c r="AA2" s="185"/>
-      <c r="AB2" s="186"/>
+      <c r="W2" s="194"/>
+      <c r="X2" s="194"/>
+      <c r="Y2" s="194"/>
+      <c r="Z2" s="194"/>
+      <c r="AA2" s="194"/>
+      <c r="AB2" s="195"/>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="95">
@@ -12048,10 +12187,10 @@
       <c r="AB26" s="5"/>
     </row>
     <row r="27" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="188" t="s">
+      <c r="A27" s="197" t="s">
         <v>228</v>
       </c>
-      <c r="B27" s="189"/>
+      <c r="B27" s="198"/>
       <c r="D27" s="110" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -12612,7 +12751,7 @@
     <mergeCell ref="A27:B27"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:AB40">
-    <cfRule type="expression" dxfId="29" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>$D3=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15679,22 +15818,22 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="D6:AA102 D3:G3 I3 D4:I5 K3:AA5">
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>$D3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J5">
-    <cfRule type="expression" dxfId="27" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>$D4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>$D3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$D3=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16405,7 +16544,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:K4">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>$D3=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16610,14 +16749,14 @@
       <c r="B14" s="20"/>
     </row>
     <row r="15" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="187" t="s">
+      <c r="B15" s="196" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="185"/>
-      <c r="D15" s="185"/>
-      <c r="E15" s="185"/>
-      <c r="F15" s="185"/>
-      <c r="G15" s="186"/>
+      <c r="C15" s="194"/>
+      <c r="D15" s="194"/>
+      <c r="E15" s="194"/>
+      <c r="F15" s="194"/>
+      <c r="G15" s="195"/>
     </row>
     <row r="16" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="105" t="s">
@@ -19619,92 +19758,92 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="U2:U18">
-    <cfRule type="expression" dxfId="23" priority="23">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>$T2="Alm_Hamre"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U18">
-    <cfRule type="expression" dxfId="22" priority="22">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>$T2="ICP_18"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U18">
-    <cfRule type="expression" dxfId="21" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$T$2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U19:U46">
-    <cfRule type="expression" dxfId="20" priority="18">
+    <cfRule type="expression" dxfId="19" priority="18">
       <formula>$T19="Alm_Hamre"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U19:U46">
-    <cfRule type="expression" dxfId="19" priority="17">
+    <cfRule type="expression" dxfId="18" priority="17">
       <formula>$T19="ICP_18"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U19:U46">
-    <cfRule type="expression" dxfId="18" priority="16">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>$T$2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U47:U51">
-    <cfRule type="expression" dxfId="17" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>$T47="Alm_Hamre"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U47:U51">
-    <cfRule type="expression" dxfId="16" priority="12">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>$T47="ICP_18"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U47:U51">
-    <cfRule type="expression" dxfId="15" priority="11">
+    <cfRule type="expression" dxfId="14" priority="11">
       <formula>$T$2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:AG18">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>$T2="Alm_Hamre"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:AG18">
-    <cfRule type="expression" dxfId="13" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>$T2="ICP_18"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:AG18">
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>$T$2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V19:AG46">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>$T19="Alm_Hamre"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V19:AG46">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$T19="ICP_18"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V19:AG46">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>$T$2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V47:AG51">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$T47="Alm_Hamre"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V47:AG51">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$T47="ICP_18"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V47:AG51">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$T$2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19745,7 +19884,7 @@
   </sheetPr>
   <dimension ref="A1:AJ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -19901,19 +20040,19 @@
       <c r="N2" s="167">
         <v>1</v>
       </c>
-      <c r="P2" s="198">
+      <c r="P2" s="185">
         <v>1</v>
       </c>
-      <c r="Q2" s="199">
-        <v>0</v>
-      </c>
-      <c r="R2" s="199">
+      <c r="Q2" s="186">
+        <v>0</v>
+      </c>
+      <c r="R2" s="186">
         <v>0.5</v>
       </c>
-      <c r="S2" s="200" t="s">
+      <c r="S2" s="187" t="s">
         <v>189</v>
       </c>
-      <c r="T2" s="195" t="s">
+      <c r="T2" s="182" t="s">
         <v>126</v>
       </c>
       <c r="U2" s="166">
@@ -19955,16 +20094,16 @@
         <f>IF(S2="Clay",AC2,AD2)</f>
         <v>1.25</v>
       </c>
-      <c r="AG2" s="201">
+      <c r="AG2" s="188">
         <v>1</v>
       </c>
-      <c r="AH2" s="195">
+      <c r="AH2" s="182">
         <v>80</v>
       </c>
       <c r="AI2" s="166">
         <v>-0.4</v>
       </c>
-      <c r="AJ2" s="193">
+      <c r="AJ2" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20002,7 +20141,7 @@
       <c r="N3" s="159">
         <v>0</v>
       </c>
-      <c r="P3" s="191">
+      <c r="P3" s="178">
         <v>2</v>
       </c>
       <c r="Q3" s="162">
@@ -20012,59 +20151,59 @@
       <c r="R3" s="162">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S3" s="197" t="s">
+      <c r="S3" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T3" s="196" t="s">
+      <c r="T3" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U3" s="192">
+      <c r="U3" s="179">
         <v>0.5</v>
       </c>
-      <c r="V3" s="192">
+      <c r="V3" s="179">
         <v>0.25</v>
       </c>
-      <c r="W3" s="192">
+      <c r="W3" s="179">
         <v>2.5</v>
       </c>
-      <c r="X3" s="192">
+      <c r="X3" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y3" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="192">
+      <c r="Y3" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="179">
         <v>9</v>
       </c>
-      <c r="AC3" s="192">
+      <c r="AC3" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD3" s="192">
+      <c r="AD3" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE3" s="192">
+      <c r="AE3" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF3" s="192">
+      <c r="AF3" s="179">
         <v>0.8</v>
       </c>
-      <c r="AG3" s="193">
+      <c r="AG3" s="180">
         <v>1</v>
       </c>
-      <c r="AH3" s="196">
+      <c r="AH3" s="183">
         <v>80</v>
       </c>
-      <c r="AI3" s="192">
+      <c r="AI3" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ3" s="193">
+      <c r="AJ3" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20090,7 +20229,7 @@
       <c r="N4" s="159">
         <v>0</v>
       </c>
-      <c r="P4" s="191">
+      <c r="P4" s="178">
         <v>3</v>
       </c>
       <c r="Q4" s="162">
@@ -20100,59 +20239,59 @@
       <c r="R4" s="162">
         <v>2</v>
       </c>
-      <c r="S4" s="197" t="s">
+      <c r="S4" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T4" s="196" t="s">
+      <c r="T4" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U4" s="192">
+      <c r="U4" s="179">
         <v>0.5</v>
       </c>
-      <c r="V4" s="192">
+      <c r="V4" s="179">
         <v>0.25</v>
       </c>
-      <c r="W4" s="192">
+      <c r="W4" s="179">
         <v>2.5</v>
       </c>
-      <c r="X4" s="192">
+      <c r="X4" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y4" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="192">
+      <c r="Y4" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="179">
         <v>9</v>
       </c>
-      <c r="AC4" s="192">
+      <c r="AC4" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD4" s="192">
+      <c r="AD4" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE4" s="192">
+      <c r="AE4" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF4" s="192">
+      <c r="AF4" s="179">
         <v>0.8</v>
       </c>
-      <c r="AG4" s="193">
+      <c r="AG4" s="180">
         <v>1</v>
       </c>
-      <c r="AH4" s="196">
+      <c r="AH4" s="183">
         <v>80</v>
       </c>
-      <c r="AI4" s="192">
+      <c r="AI4" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ4" s="193">
+      <c r="AJ4" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20178,7 +20317,7 @@
       <c r="N5" s="159">
         <v>0</v>
       </c>
-      <c r="P5" s="191">
+      <c r="P5" s="178">
         <v>4</v>
       </c>
       <c r="Q5" s="162">
@@ -20188,59 +20327,59 @@
       <c r="R5" s="162">
         <v>3.5</v>
       </c>
-      <c r="S5" s="197" t="s">
+      <c r="S5" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T5" s="196" t="s">
+      <c r="T5" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U5" s="192">
+      <c r="U5" s="179">
         <v>0.5</v>
       </c>
-      <c r="V5" s="192">
+      <c r="V5" s="179">
         <v>0.25</v>
       </c>
-      <c r="W5" s="192">
+      <c r="W5" s="179">
         <v>2.5</v>
       </c>
-      <c r="X5" s="192">
+      <c r="X5" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y5" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="192">
+      <c r="Y5" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="179">
         <v>9</v>
       </c>
-      <c r="AC5" s="192">
+      <c r="AC5" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD5" s="192">
+      <c r="AD5" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE5" s="192">
+      <c r="AE5" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF5" s="192">
+      <c r="AF5" s="179">
         <v>0.8</v>
       </c>
-      <c r="AG5" s="193">
+      <c r="AG5" s="180">
         <v>1</v>
       </c>
-      <c r="AH5" s="196">
+      <c r="AH5" s="183">
         <v>80</v>
       </c>
-      <c r="AI5" s="192">
+      <c r="AI5" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ5" s="193">
+      <c r="AJ5" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20266,7 +20405,7 @@
       <c r="N6" s="159">
         <v>0</v>
       </c>
-      <c r="P6" s="191">
+      <c r="P6" s="178">
         <v>5</v>
       </c>
       <c r="Q6" s="162">
@@ -20276,59 +20415,59 @@
       <c r="R6" s="162">
         <v>4</v>
       </c>
-      <c r="S6" s="197" t="s">
+      <c r="S6" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T6" s="196" t="s">
+      <c r="T6" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U6" s="192">
+      <c r="U6" s="179">
         <v>0.5</v>
       </c>
-      <c r="V6" s="192">
+      <c r="V6" s="179">
         <v>0.25</v>
       </c>
-      <c r="W6" s="192">
+      <c r="W6" s="179">
         <v>2.5</v>
       </c>
-      <c r="X6" s="192">
+      <c r="X6" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y6" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="192">
+      <c r="Y6" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="179">
         <v>9</v>
       </c>
-      <c r="AC6" s="192">
+      <c r="AC6" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD6" s="192">
+      <c r="AD6" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE6" s="192">
+      <c r="AE6" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF6" s="192">
+      <c r="AF6" s="179">
         <v>0.8</v>
       </c>
-      <c r="AG6" s="193">
+      <c r="AG6" s="180">
         <v>1</v>
       </c>
-      <c r="AH6" s="196">
+      <c r="AH6" s="183">
         <v>80</v>
       </c>
-      <c r="AI6" s="192">
+      <c r="AI6" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ6" s="193">
+      <c r="AJ6" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20354,7 +20493,7 @@
       <c r="N7" s="159">
         <v>0</v>
       </c>
-      <c r="P7" s="191">
+      <c r="P7" s="178">
         <v>6</v>
       </c>
       <c r="Q7" s="162">
@@ -20364,59 +20503,59 @@
       <c r="R7" s="162">
         <v>5</v>
       </c>
-      <c r="S7" s="197" t="s">
+      <c r="S7" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="T7" s="196" t="s">
+      <c r="T7" s="183" t="s">
         <v>295</v>
       </c>
-      <c r="U7" s="192">
+      <c r="U7" s="179">
         <v>0.5</v>
       </c>
-      <c r="V7" s="192">
+      <c r="V7" s="179">
         <v>0.25</v>
       </c>
-      <c r="W7" s="192">
+      <c r="W7" s="179">
         <v>2.5</v>
       </c>
-      <c r="X7" s="192">
+      <c r="X7" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y7" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="192">
+      <c r="Y7" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="179">
         <v>9</v>
       </c>
-      <c r="AC7" s="192">
+      <c r="AC7" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD7" s="192">
+      <c r="AD7" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE7" s="192">
+      <c r="AE7" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF7" s="192">
+      <c r="AF7" s="179">
         <v>0.8</v>
       </c>
-      <c r="AG7" s="193">
+      <c r="AG7" s="180">
         <v>1</v>
       </c>
-      <c r="AH7" s="196">
+      <c r="AH7" s="183">
         <v>80</v>
       </c>
-      <c r="AI7" s="192">
+      <c r="AI7" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ7" s="193">
+      <c r="AJ7" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20442,7 +20581,7 @@
       <c r="N8" s="159">
         <v>0</v>
       </c>
-      <c r="P8" s="191">
+      <c r="P8" s="178">
         <v>7</v>
       </c>
       <c r="Q8" s="162">
@@ -20452,59 +20591,59 @@
       <c r="R8" s="162">
         <v>5.9</v>
       </c>
-      <c r="S8" s="197" t="s">
+      <c r="S8" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="T8" s="196" t="s">
+      <c r="T8" s="183" t="s">
         <v>295</v>
       </c>
-      <c r="U8" s="192">
+      <c r="U8" s="179">
         <v>0.5</v>
       </c>
-      <c r="V8" s="192">
+      <c r="V8" s="179">
         <v>0.25</v>
       </c>
-      <c r="W8" s="192">
+      <c r="W8" s="179">
         <v>2.5</v>
       </c>
-      <c r="X8" s="192">
+      <c r="X8" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y8" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="192">
+      <c r="Y8" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="179">
         <v>9</v>
       </c>
-      <c r="AC8" s="192">
+      <c r="AC8" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD8" s="192">
+      <c r="AD8" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE8" s="192">
+      <c r="AE8" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF8" s="192">
+      <c r="AF8" s="179">
         <v>0.8</v>
       </c>
-      <c r="AG8" s="193">
+      <c r="AG8" s="180">
         <v>1</v>
       </c>
-      <c r="AH8" s="196">
+      <c r="AH8" s="183">
         <v>80</v>
       </c>
-      <c r="AI8" s="192">
+      <c r="AI8" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ8" s="193">
+      <c r="AJ8" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20530,7 +20669,7 @@
       <c r="N9" s="159">
         <v>0</v>
       </c>
-      <c r="P9" s="191">
+      <c r="P9" s="178">
         <v>8</v>
       </c>
       <c r="Q9" s="162">
@@ -20540,59 +20679,59 @@
       <c r="R9" s="162">
         <v>10.9</v>
       </c>
-      <c r="S9" s="197" t="s">
+      <c r="S9" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T9" s="196" t="s">
+      <c r="T9" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U9" s="192">
+      <c r="U9" s="179">
         <v>0.5</v>
       </c>
-      <c r="V9" s="192">
+      <c r="V9" s="179">
         <v>0.25</v>
       </c>
-      <c r="W9" s="192">
+      <c r="W9" s="179">
         <v>2.5</v>
       </c>
-      <c r="X9" s="192">
+      <c r="X9" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y9" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="192">
+      <c r="Y9" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="179">
         <v>9</v>
       </c>
-      <c r="AC9" s="192">
+      <c r="AC9" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD9" s="192">
+      <c r="AD9" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE9" s="192">
+      <c r="AE9" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF9" s="192">
+      <c r="AF9" s="179">
         <v>0.8</v>
       </c>
-      <c r="AG9" s="193">
+      <c r="AG9" s="180">
         <v>1</v>
       </c>
-      <c r="AH9" s="196">
+      <c r="AH9" s="183">
         <v>80</v>
       </c>
-      <c r="AI9" s="192">
+      <c r="AI9" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ9" s="193">
+      <c r="AJ9" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20618,7 +20757,7 @@
       <c r="N10" s="159">
         <v>0</v>
       </c>
-      <c r="P10" s="191">
+      <c r="P10" s="178">
         <v>9</v>
       </c>
       <c r="Q10" s="162">
@@ -20628,59 +20767,59 @@
       <c r="R10" s="162">
         <v>14</v>
       </c>
-      <c r="S10" s="197" t="s">
+      <c r="S10" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T10" s="196" t="s">
+      <c r="T10" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U10" s="192">
+      <c r="U10" s="179">
         <v>0.5</v>
       </c>
-      <c r="V10" s="192">
+      <c r="V10" s="179">
         <v>0.25</v>
       </c>
-      <c r="W10" s="192">
+      <c r="W10" s="179">
         <v>2.5</v>
       </c>
-      <c r="X10" s="192">
+      <c r="X10" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y10" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="192">
+      <c r="Y10" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="179">
         <v>9</v>
       </c>
-      <c r="AC10" s="192">
+      <c r="AC10" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD10" s="192">
+      <c r="AD10" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE10" s="192">
+      <c r="AE10" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF10" s="192">
+      <c r="AF10" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG10" s="193">
+      <c r="AG10" s="180">
         <v>1</v>
       </c>
-      <c r="AH10" s="196">
+      <c r="AH10" s="183">
         <v>80</v>
       </c>
-      <c r="AI10" s="192">
+      <c r="AI10" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ10" s="193">
+      <c r="AJ10" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20706,7 +20845,7 @@
       <c r="N11" s="159">
         <v>0</v>
       </c>
-      <c r="P11" s="191">
+      <c r="P11" s="178">
         <v>10</v>
       </c>
       <c r="Q11" s="162">
@@ -20716,59 +20855,59 @@
       <c r="R11" s="162">
         <v>16.5</v>
       </c>
-      <c r="S11" s="197" t="s">
+      <c r="S11" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T11" s="196" t="s">
+      <c r="T11" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U11" s="192">
+      <c r="U11" s="179">
         <v>0.5</v>
       </c>
-      <c r="V11" s="192">
+      <c r="V11" s="179">
         <v>0.25</v>
       </c>
-      <c r="W11" s="192">
+      <c r="W11" s="179">
         <v>2.5</v>
       </c>
-      <c r="X11" s="192">
+      <c r="X11" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y11" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="192">
+      <c r="Y11" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="179">
         <v>9</v>
       </c>
-      <c r="AC11" s="192">
+      <c r="AC11" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD11" s="192">
+      <c r="AD11" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE11" s="192">
+      <c r="AE11" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF11" s="192">
+      <c r="AF11" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG11" s="193">
+      <c r="AG11" s="180">
         <v>1</v>
       </c>
-      <c r="AH11" s="196">
+      <c r="AH11" s="183">
         <v>80</v>
       </c>
-      <c r="AI11" s="192">
+      <c r="AI11" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ11" s="193">
+      <c r="AJ11" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20794,7 +20933,7 @@
       <c r="N12" s="159">
         <v>0</v>
       </c>
-      <c r="P12" s="191">
+      <c r="P12" s="178">
         <v>11</v>
       </c>
       <c r="Q12" s="162">
@@ -20804,59 +20943,59 @@
       <c r="R12" s="162">
         <v>19.8</v>
       </c>
-      <c r="S12" s="197" t="s">
+      <c r="S12" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T12" s="196" t="s">
+      <c r="T12" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U12" s="192">
+      <c r="U12" s="179">
         <v>0.5</v>
       </c>
-      <c r="V12" s="192">
+      <c r="V12" s="179">
         <v>0.25</v>
       </c>
-      <c r="W12" s="192">
+      <c r="W12" s="179">
         <v>2.5</v>
       </c>
-      <c r="X12" s="192">
+      <c r="X12" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y12" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="192">
+      <c r="Y12" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="179">
         <v>9</v>
       </c>
-      <c r="AC12" s="192">
+      <c r="AC12" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD12" s="192">
+      <c r="AD12" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE12" s="192">
+      <c r="AE12" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF12" s="192">
+      <c r="AF12" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG12" s="193">
+      <c r="AG12" s="180">
         <v>1</v>
       </c>
-      <c r="AH12" s="196">
+      <c r="AH12" s="183">
         <v>80</v>
       </c>
-      <c r="AI12" s="192">
+      <c r="AI12" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ12" s="193">
+      <c r="AJ12" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20882,7 +21021,7 @@
       <c r="N13" s="159">
         <v>0</v>
       </c>
-      <c r="P13" s="191">
+      <c r="P13" s="178">
         <v>12</v>
       </c>
       <c r="Q13" s="162">
@@ -20892,59 +21031,59 @@
       <c r="R13" s="162">
         <v>30</v>
       </c>
-      <c r="S13" s="197" t="s">
+      <c r="S13" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="T13" s="196" t="s">
+      <c r="T13" s="183" t="s">
         <v>295</v>
       </c>
-      <c r="U13" s="192">
+      <c r="U13" s="179">
         <v>0.5</v>
       </c>
-      <c r="V13" s="192">
+      <c r="V13" s="179">
         <v>0.25</v>
       </c>
-      <c r="W13" s="192">
+      <c r="W13" s="179">
         <v>2.5</v>
       </c>
-      <c r="X13" s="192">
+      <c r="X13" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y13" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="192">
+      <c r="Y13" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="179">
         <v>9</v>
       </c>
-      <c r="AC13" s="192">
+      <c r="AC13" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD13" s="192">
+      <c r="AD13" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE13" s="192">
+      <c r="AE13" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF13" s="192">
+      <c r="AF13" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG13" s="193">
+      <c r="AG13" s="180">
         <v>1</v>
       </c>
-      <c r="AH13" s="196">
+      <c r="AH13" s="183">
         <v>80</v>
       </c>
-      <c r="AI13" s="192">
+      <c r="AI13" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ13" s="193">
+      <c r="AJ13" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -20971,7 +21110,7 @@
       <c r="N14" s="163">
         <v>0</v>
       </c>
-      <c r="P14" s="191">
+      <c r="P14" s="178">
         <v>13</v>
       </c>
       <c r="Q14" s="162">
@@ -20981,59 +21120,59 @@
       <c r="R14" s="162">
         <v>42.8</v>
       </c>
-      <c r="S14" s="197" t="s">
+      <c r="S14" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="T14" s="196" t="s">
+      <c r="T14" s="183" t="s">
         <v>295</v>
       </c>
-      <c r="U14" s="192">
+      <c r="U14" s="179">
         <v>0.5</v>
       </c>
-      <c r="V14" s="192">
+      <c r="V14" s="179">
         <v>0.25</v>
       </c>
-      <c r="W14" s="192">
+      <c r="W14" s="179">
         <v>2.5</v>
       </c>
-      <c r="X14" s="192">
+      <c r="X14" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y14" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="192">
+      <c r="Y14" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="179">
         <v>9</v>
       </c>
-      <c r="AC14" s="192">
+      <c r="AC14" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD14" s="192">
+      <c r="AD14" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE14" s="192">
+      <c r="AE14" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF14" s="192">
+      <c r="AF14" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG14" s="193">
+      <c r="AG14" s="180">
         <v>1</v>
       </c>
-      <c r="AH14" s="196">
+      <c r="AH14" s="183">
         <v>80</v>
       </c>
-      <c r="AI14" s="192">
+      <c r="AI14" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ14" s="193">
+      <c r="AJ14" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -21050,7 +21189,7 @@
       <c r="J15" s="159" t="s">
         <v>167</v>
       </c>
-      <c r="P15" s="191">
+      <c r="P15" s="178">
         <v>14</v>
       </c>
       <c r="Q15" s="162">
@@ -21060,59 +21199,59 @@
       <c r="R15" s="162">
         <v>47.5</v>
       </c>
-      <c r="S15" s="197" t="s">
+      <c r="S15" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="T15" s="196" t="s">
+      <c r="T15" s="183" t="s">
         <v>126</v>
       </c>
-      <c r="U15" s="192">
+      <c r="U15" s="179">
         <v>0.5</v>
       </c>
-      <c r="V15" s="192">
+      <c r="V15" s="179">
         <v>0.25</v>
       </c>
-      <c r="W15" s="192">
+      <c r="W15" s="179">
         <v>2.5</v>
       </c>
-      <c r="X15" s="192">
+      <c r="X15" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y15" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="192">
+      <c r="Y15" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="179">
         <v>9</v>
       </c>
-      <c r="AC15" s="192">
+      <c r="AC15" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD15" s="192">
+      <c r="AD15" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE15" s="192">
+      <c r="AE15" s="179">
         <f t="shared" si="0"/>
         <v>3.6176470588235294</v>
       </c>
-      <c r="AF15" s="192">
+      <c r="AF15" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG15" s="193">
+      <c r="AG15" s="180">
         <v>1</v>
       </c>
-      <c r="AH15" s="196">
+      <c r="AH15" s="183">
         <v>80</v>
       </c>
-      <c r="AI15" s="192">
+      <c r="AI15" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ15" s="193">
+      <c r="AJ15" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -21129,7 +21268,7 @@
       <c r="J16" s="159" t="s">
         <v>167</v>
       </c>
-      <c r="P16" s="191">
+      <c r="P16" s="178">
         <v>15</v>
       </c>
       <c r="Q16" s="162">
@@ -21139,58 +21278,58 @@
       <c r="R16" s="162">
         <v>55</v>
       </c>
-      <c r="S16" s="197" t="s">
+      <c r="S16" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="T16" s="196" t="s">
+      <c r="T16" s="183" t="s">
         <v>295</v>
       </c>
-      <c r="U16" s="192">
+      <c r="U16" s="179">
         <v>0.5</v>
       </c>
-      <c r="V16" s="192">
+      <c r="V16" s="179">
         <v>0.25</v>
       </c>
-      <c r="W16" s="192">
+      <c r="W16" s="179">
         <v>2.5</v>
       </c>
-      <c r="X16" s="192">
+      <c r="X16" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y16" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="192">
+      <c r="Y16" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="179">
         <v>9</v>
       </c>
-      <c r="AC16" s="192">
+      <c r="AC16" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD16" s="192">
+      <c r="AD16" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE16" s="192">
+      <c r="AE16" s="179">
         <v>1.5</v>
       </c>
-      <c r="AF16" s="192">
+      <c r="AF16" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG16" s="193">
+      <c r="AG16" s="180">
         <v>1</v>
       </c>
-      <c r="AH16" s="196">
+      <c r="AH16" s="183">
         <v>80</v>
       </c>
-      <c r="AI16" s="192">
+      <c r="AI16" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ16" s="193">
+      <c r="AJ16" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -21207,7 +21346,7 @@
       <c r="J17" s="159" t="s">
         <v>167</v>
       </c>
-      <c r="P17" s="191">
+      <c r="P17" s="178">
         <v>16</v>
       </c>
       <c r="Q17" s="162">
@@ -21217,58 +21356,58 @@
       <c r="R17" s="162">
         <v>61</v>
       </c>
-      <c r="S17" s="197" t="s">
+      <c r="S17" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="T17" s="196" t="s">
+      <c r="T17" s="183" t="s">
         <v>295</v>
       </c>
-      <c r="U17" s="192">
+      <c r="U17" s="179">
         <v>0.5</v>
       </c>
-      <c r="V17" s="192">
+      <c r="V17" s="179">
         <v>0.25</v>
       </c>
-      <c r="W17" s="192">
+      <c r="W17" s="179">
         <v>2.5</v>
       </c>
-      <c r="X17" s="192">
+      <c r="X17" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y17" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="192">
+      <c r="Y17" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="179">
         <v>9</v>
       </c>
-      <c r="AC17" s="192">
+      <c r="AC17" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD17" s="192">
+      <c r="AD17" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE17" s="192">
+      <c r="AE17" s="179">
         <v>1.5</v>
       </c>
-      <c r="AF17" s="192">
+      <c r="AF17" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG17" s="193">
+      <c r="AG17" s="180">
         <v>1</v>
       </c>
-      <c r="AH17" s="196">
+      <c r="AH17" s="183">
         <v>80</v>
       </c>
-      <c r="AI17" s="192">
+      <c r="AI17" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ17" s="193">
+      <c r="AJ17" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -21285,68 +21424,68 @@
       <c r="J18" s="159" t="s">
         <v>167</v>
       </c>
-      <c r="P18" s="194">
+      <c r="P18" s="181">
         <v>17</v>
       </c>
-      <c r="Q18" s="190">
+      <c r="Q18" s="177">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="R18" s="190">
+      <c r="R18" s="177">
         <v>80</v>
       </c>
-      <c r="S18" s="197" t="s">
+      <c r="S18" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="T18" s="196" t="s">
+      <c r="T18" s="183" t="s">
         <v>295</v>
       </c>
-      <c r="U18" s="192">
+      <c r="U18" s="179">
         <v>0.5</v>
       </c>
-      <c r="V18" s="192">
+      <c r="V18" s="179">
         <v>0.25</v>
       </c>
-      <c r="W18" s="192">
+      <c r="W18" s="179">
         <v>2.5</v>
       </c>
-      <c r="X18" s="192">
+      <c r="X18" s="179">
         <v>2.5</v>
       </c>
-      <c r="Y18" s="192">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="192">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="192">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="192">
+      <c r="Y18" s="179">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="179">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="179">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="179">
         <v>9</v>
       </c>
-      <c r="AC18" s="192">
+      <c r="AC18" s="179">
         <v>0.8</v>
       </c>
-      <c r="AD18" s="192">
+      <c r="AD18" s="179">
         <v>1.25</v>
       </c>
-      <c r="AE18" s="192">
+      <c r="AE18" s="179">
         <v>1.5</v>
       </c>
-      <c r="AF18" s="192">
+      <c r="AF18" s="179">
         <v>1.25</v>
       </c>
-      <c r="AG18" s="193">
+      <c r="AG18" s="180">
         <v>1</v>
       </c>
-      <c r="AH18" s="196">
+      <c r="AH18" s="183">
         <v>80</v>
       </c>
-      <c r="AI18" s="192">
+      <c r="AI18" s="179">
         <v>-0.4</v>
       </c>
-      <c r="AJ18" s="193">
+      <c r="AJ18" s="180">
         <v>0.3</v>
       </c>
     </row>
@@ -22651,27 +22790,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Y2:AB18">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$T2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:X18">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$T2="Alm_Hamre"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:X18">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$T2="ICP_18"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:X18">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$T$2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AE18 AG2:AH18 AJ2:AJ18">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$T2="Stevens"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>